<commit_message>
Update Create Multiple on Question Result
</commit_message>
<xml_diff>
--- a/backend/src/data/test_norma.xlsx
+++ b/backend/src/data/test_norma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Important Files\Informatika ISTTS\_Semester 6\Kerja_Praktek\Project\adiputro_psytest_backend\backend\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9660FB-B149-49D3-8665-71C1493C3425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD01BE1-192D-402C-A6C6-09EE083C0CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="10" xr2:uid="{28313136-274B-432F-8942-0592E5394583}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{28313136-274B-432F-8942-0592E5394583}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="11" r:id="rId1"/>
@@ -222,9 +222,6 @@
     <t>20-29</t>
   </si>
   <si>
-    <t>30-50</t>
-  </si>
-  <si>
     <t>48-50</t>
   </si>
   <si>
@@ -289,6 +286,9 @@
   </si>
   <si>
     <t>2-5</t>
+  </si>
+  <si>
+    <t>30-38</t>
   </si>
 </sst>
 </file>
@@ -2110,7 +2110,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="54">
         <v>5</v>
@@ -2126,7 +2126,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="50" t="s">
         <v>37</v>
@@ -2134,7 +2134,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="50" t="s">
         <v>36</v>
@@ -2142,7 +2142,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="50" t="s">
         <v>35</v>
@@ -2150,7 +2150,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="50" t="s">
         <v>34</v>
@@ -2158,7 +2158,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="50" t="s">
         <v>33</v>
@@ -2173,7 +2173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D471B223-FE94-40E2-BCDA-46194F85E0A6}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -2181,7 +2181,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="54">
         <v>5</v>
@@ -2197,7 +2197,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="54" t="s">
         <v>37</v>
@@ -2205,7 +2205,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="55" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="54" t="s">
         <v>36</v>
@@ -2213,7 +2213,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="54" t="s">
         <v>35</v>
@@ -2221,7 +2221,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="54" t="s">
         <v>34</v>
@@ -2229,7 +2229,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="54" t="s">
         <v>33</v>
@@ -8029,7 +8029,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="54">
         <v>5</v>
@@ -8093,15 +8093,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99833A5E-DEDE-4459-AE5F-47EE96DED0B4}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="54">
         <v>5</v>
@@ -8117,7 +8117,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>37</v>
@@ -8172,7 +8172,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="54">
         <v>5</v>
@@ -8188,7 +8188,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="31" t="s">
         <v>37</v>
@@ -8196,7 +8196,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="31" t="s">
         <v>36</v>
@@ -8204,7 +8204,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>35</v>
@@ -8212,7 +8212,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" s="31" t="s">
         <v>34</v>
@@ -8220,7 +8220,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="31" t="s">
         <v>33</v>
@@ -8243,7 +8243,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="54">
         <v>5</v>
@@ -8259,7 +8259,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="34" t="s">
         <v>37</v>
@@ -8267,7 +8267,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="34" t="s">
         <v>36</v>
@@ -8275,7 +8275,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="34" t="s">
         <v>35</v>
@@ -8283,7 +8283,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="34" t="s">
         <v>34</v>
@@ -8291,7 +8291,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="55" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="54" t="s">
         <v>33</v>
@@ -8314,7 +8314,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="54">
         <v>5</v>
@@ -8330,7 +8330,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="38" t="s">
         <v>37</v>
@@ -8385,7 +8385,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="54">
         <v>5</v>
@@ -8401,7 +8401,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="42" t="s">
         <v>37</v>
@@ -8409,7 +8409,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="42" t="s">
         <v>36</v>
@@ -8417,7 +8417,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="42" t="s">
         <v>35</v>
@@ -8425,7 +8425,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" s="42" t="s">
         <v>34</v>
@@ -8433,7 +8433,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="42" t="s">
         <v>33</v>
@@ -8456,7 +8456,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="54">
         <v>5</v>
@@ -8472,7 +8472,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="46" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
update other test page design
</commit_message>
<xml_diff>
--- a/backend/src/data/test_norma.xlsx
+++ b/backend/src/data/test_norma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Important Files\Informatika ISTTS\_Semester 6\Kerja_Praktek\Project\adiputro_psytest_backend\backend\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\adiputro_psytest_backend\backend\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD01BE1-192D-402C-A6C6-09EE083C0CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2236C520-9587-4CB4-B75F-5EC9370AE7EF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{28313136-274B-432F-8942-0592E5394583}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11316" activeTab="7" xr2:uid="{28313136-274B-432F-8942-0592E5394583}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="11" r:id="rId1"/>
@@ -25,18 +25,10 @@
     <sheet name="14" sheetId="8" r:id="rId10"/>
     <sheet name="15" sheetId="9" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -258,9 +250,6 @@
     <t>36-47</t>
   </si>
   <si>
-    <t>35-24</t>
-  </si>
-  <si>
     <t>12-23</t>
   </si>
   <si>
@@ -289,6 +278,9 @@
   </si>
   <si>
     <t>30-38</t>
+  </si>
+  <si>
+    <t>24-35</t>
   </si>
 </sst>
 </file>
@@ -943,9 +935,9 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B1" s="20" t="s">
         <v>21</v>
       </c>
@@ -983,7 +975,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="20">
         <v>0</v>
       </c>
@@ -1024,7 +1016,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -1068,7 +1060,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="20">
         <f>A3+1</f>
         <v>2</v>
@@ -1117,7 +1109,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="20">
         <f t="shared" ref="A5:A22" si="0">A4+1</f>
         <v>3</v>
@@ -1163,7 +1155,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="20">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1215,7 +1207,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="20">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1261,7 +1253,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="20">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1307,7 +1299,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="20">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1353,7 +1345,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="20">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1399,7 +1391,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="20">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1445,7 +1437,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="20">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1491,7 +1483,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="20">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1534,7 +1526,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="20">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1580,7 +1572,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="20">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1620,7 +1612,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="20">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1660,7 +1652,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="20">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1700,7 +1692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="20">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1740,7 +1732,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="20">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1780,7 +1772,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="20">
         <f>A19+1</f>
         <v>18</v>
@@ -1817,7 +1809,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1854,7 +1846,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="20">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1886,7 +1878,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1930,7 +1922,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="23" t="s">
         <v>41</v>
       </c>
@@ -1965,7 +1957,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -2022,7 +2014,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -2071,13 +2063,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="23"/>
       <c r="B29" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -2085,7 +2077,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -2106,17 +2098,17 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="54">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="52" t="s">
         <v>49</v>
       </c>
@@ -2124,41 +2116,41 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="50" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="50" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="53" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" s="50" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" s="50" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7" s="50" t="s">
         <v>33</v>
@@ -2177,17 +2169,17 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="54">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="56" t="s">
         <v>49</v>
       </c>
@@ -2195,41 +2187,41 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="54" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="55" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="54" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="57" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" s="54" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="55" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" s="54" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7" s="54" t="s">
         <v>33</v>
@@ -2248,9 +2240,9 @@
       <selection activeCell="BP31" sqref="BP31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2328,7 +2320,7 @@
       <c r="BO1" s="1"/>
       <c r="BP1" s="1"/>
     </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2534,7 +2526,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>0</v>
       </c>
@@ -2616,7 +2608,7 @@
       <c r="BO3" s="16"/>
       <c r="BP3" s="16"/>
     </row>
-    <row r="4" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -2710,7 +2702,7 @@
       <c r="BO4" s="16"/>
       <c r="BP4" s="16"/>
     </row>
-    <row r="5" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -2816,7 +2808,7 @@
       </c>
       <c r="BP5" s="16"/>
     </row>
-    <row r="6" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -2948,7 +2940,7 @@
       </c>
       <c r="BP6" s="16"/>
     </row>
-    <row r="7" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>4</v>
       </c>
@@ -3102,7 +3094,7 @@
       </c>
       <c r="BP7" s="16"/>
     </row>
-    <row r="8" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -3284,7 +3276,7 @@
       </c>
       <c r="BP8" s="16"/>
     </row>
-    <row r="9" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -3480,7 +3472,7 @@
       </c>
       <c r="BP9" s="16"/>
     </row>
-    <row r="10" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>7</v>
       </c>
@@ -3686,7 +3678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>8</v>
       </c>
@@ -3892,7 +3884,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>9</v>
       </c>
@@ -4098,7 +4090,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>10</v>
       </c>
@@ -4304,7 +4296,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>11</v>
       </c>
@@ -4510,7 +4502,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>12</v>
       </c>
@@ -4716,7 +4708,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>13</v>
       </c>
@@ -4922,7 +4914,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>14</v>
       </c>
@@ -5128,7 +5120,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>15</v>
       </c>
@@ -5334,7 +5326,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>16</v>
       </c>
@@ -5540,7 +5532,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>17</v>
       </c>
@@ -5746,7 +5738,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>18</v>
       </c>
@@ -5952,7 +5944,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>19</v>
       </c>
@@ -6158,7 +6150,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>20</v>
       </c>
@@ -6364,7 +6356,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>21</v>
       </c>
@@ -6570,7 +6562,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>22</v>
       </c>
@@ -6776,7 +6768,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>23</v>
       </c>
@@ -6982,7 +6974,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>24</v>
       </c>
@@ -7188,7 +7180,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>25</v>
       </c>
@@ -7394,7 +7386,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>26</v>
       </c>
@@ -7600,7 +7592,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>27</v>
       </c>
@@ -7806,7 +7798,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>28</v>
       </c>
@@ -8025,17 +8017,17 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="54">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>49</v>
       </c>
@@ -8043,7 +8035,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>50</v>
       </c>
@@ -8051,7 +8043,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>51</v>
       </c>
@@ -8059,7 +8051,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
         <v>52</v>
       </c>
@@ -8067,7 +8059,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
         <v>53</v>
       </c>
@@ -8075,7 +8067,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>54</v>
       </c>
@@ -8093,21 +8085,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99833A5E-DEDE-4459-AE5F-47EE96DED0B4}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="54">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>49</v>
       </c>
@@ -8115,15 +8107,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>58</v>
       </c>
@@ -8131,7 +8123,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
         <v>57</v>
       </c>
@@ -8139,7 +8131,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
         <v>56</v>
       </c>
@@ -8147,7 +8139,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>54</v>
       </c>
@@ -8168,17 +8160,17 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="54">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
         <v>49</v>
       </c>
@@ -8186,7 +8178,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>59</v>
       </c>
@@ -8194,7 +8186,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
         <v>60</v>
       </c>
@@ -8202,7 +8194,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
         <v>61</v>
       </c>
@@ -8210,7 +8202,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
         <v>62</v>
       </c>
@@ -8218,7 +8210,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>63</v>
       </c>
@@ -8239,17 +8231,17 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="54">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
         <v>49</v>
       </c>
@@ -8257,7 +8249,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
         <v>64</v>
       </c>
@@ -8265,7 +8257,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
         <v>65</v>
       </c>
@@ -8273,7 +8265,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="37" t="s">
         <v>66</v>
       </c>
@@ -8281,7 +8273,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="35" t="s">
         <v>67</v>
       </c>
@@ -8289,9 +8281,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="54" t="s">
         <v>33</v>
@@ -8310,17 +8302,17 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="54">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>49</v>
       </c>
@@ -8328,7 +8320,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="41" t="s">
         <v>68</v>
       </c>
@@ -8336,7 +8328,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="39" t="s">
         <v>51</v>
       </c>
@@ -8344,7 +8336,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="41" t="s">
         <v>52</v>
       </c>
@@ -8352,7 +8344,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="55" t="s">
         <v>53</v>
       </c>
@@ -8360,7 +8352,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="57" t="s">
         <v>54</v>
       </c>
@@ -8377,21 +8369,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B2F4E0-04ED-4419-995D-BAD7964855D3}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="54">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="44" t="s">
         <v>49</v>
       </c>
@@ -8399,7 +8391,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="45" t="s">
         <v>69</v>
       </c>
@@ -8407,7 +8399,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="43" t="s">
         <v>70</v>
       </c>
@@ -8415,25 +8407,25 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
-        <v>71</v>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="57" t="s">
+        <v>81</v>
       </c>
       <c r="B5" s="42" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="42" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" s="42" t="s">
         <v>33</v>
@@ -8452,17 +8444,17 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="54">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
         <v>49</v>
       </c>
@@ -8470,7 +8462,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="49" t="s">
         <v>68</v>
       </c>
@@ -8478,7 +8470,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>51</v>
       </c>
@@ -8486,7 +8478,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="49" t="s">
         <v>52</v>
       </c>
@@ -8494,7 +8486,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>53</v>
       </c>
@@ -8502,7 +8494,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="49" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Insert Question From Excel + Add IST, Akudak, Hafalan Questions
</commit_message>
<xml_diff>
--- a/backend/src/data/test_norma.xlsx
+++ b/backend/src/data/test_norma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Important Files\Informatika ISTTS\_Semester 6\Kerja_Praktek\Project\adiputro_psytest_backend\backend\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D29024-B76C-4CDC-988D-72A5AE27109D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7110767C-18FC-4D9A-8FB6-6B2C60B229AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{28313136-274B-432F-8942-0592E5394583}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="3" activeTab="16" xr2:uid="{28313136-274B-432F-8942-0592E5394583}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="11" r:id="rId1"/>
@@ -22,11 +22,14 @@
     <sheet name="7" sheetId="2" r:id="rId7"/>
     <sheet name="8" sheetId="3" r:id="rId8"/>
     <sheet name="9" sheetId="4" r:id="rId9"/>
-    <sheet name="11" sheetId="5" r:id="rId10"/>
-    <sheet name="12" sheetId="6" r:id="rId11"/>
-    <sheet name="13" sheetId="7" r:id="rId12"/>
-    <sheet name="14" sheetId="8" r:id="rId13"/>
-    <sheet name="15" sheetId="9" r:id="rId14"/>
+    <sheet name="10" sheetId="15" r:id="rId10"/>
+    <sheet name="11" sheetId="5" r:id="rId11"/>
+    <sheet name="12" sheetId="6" r:id="rId12"/>
+    <sheet name="13" sheetId="7" r:id="rId13"/>
+    <sheet name="14" sheetId="8" r:id="rId14"/>
+    <sheet name="15" sheetId="9" r:id="rId15"/>
+    <sheet name="17" sheetId="16" r:id="rId16"/>
+    <sheet name="21" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -46,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="242">
   <si>
     <t>College Student (Men)</t>
   </si>
@@ -550,13 +553,235 @@
   </si>
   <si>
     <t>13-52</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>16-20</t>
+  </si>
+  <si>
+    <t>21-24</t>
+  </si>
+  <si>
+    <t>3-6</t>
+  </si>
+  <si>
+    <t>12-15</t>
+  </si>
+  <si>
+    <t>25-299</t>
+  </si>
+  <si>
+    <t>30-33</t>
+  </si>
+  <si>
+    <t>34-38</t>
+  </si>
+  <si>
+    <t>39-42</t>
+  </si>
+  <si>
+    <t>43-46</t>
+  </si>
+  <si>
+    <t>47-51</t>
+  </si>
+  <si>
+    <t>52-55</t>
+  </si>
+  <si>
+    <t>56-60</t>
+  </si>
+  <si>
+    <t>61-64</t>
+  </si>
+  <si>
+    <t>65-68</t>
+  </si>
+  <si>
+    <t>69-73</t>
+  </si>
+  <si>
+    <t>78-80</t>
+  </si>
+  <si>
+    <t>74-77</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>0-16</t>
+  </si>
+  <si>
+    <t>17-17</t>
+  </si>
+  <si>
+    <t>18-19</t>
+  </si>
+  <si>
+    <t>20-20</t>
+  </si>
+  <si>
+    <t>21-22</t>
+  </si>
+  <si>
+    <t>23-24</t>
+  </si>
+  <si>
+    <t>25-25</t>
+  </si>
+  <si>
+    <t>26-27</t>
+  </si>
+  <si>
+    <t>28-29</t>
+  </si>
+  <si>
+    <t>30-30</t>
+  </si>
+  <si>
+    <t>31-32</t>
+  </si>
+  <si>
+    <t>33-34</t>
+  </si>
+  <si>
+    <t>35-35</t>
+  </si>
+  <si>
+    <t>36-37</t>
+  </si>
+  <si>
+    <t>38-39</t>
+  </si>
+  <si>
+    <t>40-40</t>
+  </si>
+  <si>
+    <t>41-42</t>
+  </si>
+  <si>
+    <t>43-44</t>
+  </si>
+  <si>
+    <t>45-45</t>
+  </si>
+  <si>
+    <t>46-47</t>
+  </si>
+  <si>
+    <t>5-5</t>
+  </si>
+  <si>
+    <t>6-6</t>
+  </si>
+  <si>
+    <t>7-7</t>
+  </si>
+  <si>
+    <t>8-8</t>
+  </si>
+  <si>
+    <t>9-9</t>
+  </si>
+  <si>
+    <t>11-11</t>
+  </si>
+  <si>
+    <t>9-10</t>
+  </si>
+  <si>
+    <t>13-13</t>
+  </si>
+  <si>
+    <t>14-14</t>
+  </si>
+  <si>
+    <t>15-15</t>
+  </si>
+  <si>
+    <t>16-16</t>
+  </si>
+  <si>
+    <t>18-18</t>
+  </si>
+  <si>
+    <t>19-19</t>
+  </si>
+  <si>
+    <t>21-25</t>
+  </si>
+  <si>
+    <t>16-17</t>
+  </si>
+  <si>
+    <t>19-20</t>
+  </si>
+  <si>
+    <t>21-21</t>
+  </si>
+  <si>
+    <t>22-23</t>
+  </si>
+  <si>
+    <t>24-24</t>
+  </si>
+  <si>
+    <t>28-28</t>
+  </si>
+  <si>
+    <t>29-30</t>
+  </si>
+  <si>
+    <t>31-31</t>
+  </si>
+  <si>
+    <t>32-33</t>
+  </si>
+  <si>
+    <t>34-34</t>
+  </si>
+  <si>
+    <t>35-36</t>
+  </si>
+  <si>
+    <t>37-37</t>
+  </si>
+  <si>
+    <t>15-16</t>
+  </si>
+  <si>
+    <t>25-26</t>
+  </si>
+  <si>
+    <t>27-27</t>
+  </si>
+  <si>
+    <t>31-40</t>
+  </si>
+  <si>
+    <t>0-4,9</t>
+  </si>
+  <si>
+    <t>8-999</t>
+  </si>
+  <si>
+    <t>5-5,9</t>
+  </si>
+  <si>
+    <t>6-6,9</t>
+  </si>
+  <si>
+    <t>7-7,9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -594,6 +819,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="14">
@@ -777,7 +1008,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -951,6 +1182,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1273,7 +1505,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -2433,12 +2665,773 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E425E2-BA8B-44FA-A16E-BB1E0B68198A}">
+  <dimension ref="A1:Q23"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="74"/>
+    <col min="7" max="7" width="9.140625" style="74"/>
+    <col min="10" max="10" width="9.140625" style="74"/>
+    <col min="13" max="13" width="9.140625" style="74"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="76" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="D1" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="56"/>
+      <c r="G1" s="76" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="56"/>
+      <c r="J1" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="56"/>
+      <c r="M1" s="76" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="56"/>
+      <c r="P1" s="76" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q1" s="54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="G2" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="J2" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="K2" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="M2" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="N2" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="P2" s="76" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" s="56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="74" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="74" t="s">
+        <v>120</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="P3" s="75" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q3" s="54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4" s="54">
+        <v>1</v>
+      </c>
+      <c r="G4" s="74" t="s">
+        <v>207</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="M4" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="P4" s="75" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q4" s="54" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="74" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="54">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" s="54">
+        <v>2</v>
+      </c>
+      <c r="G5" s="74" t="s">
+        <v>208</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="J5" s="74" t="s">
+        <v>145</v>
+      </c>
+      <c r="K5" s="54">
+        <v>2</v>
+      </c>
+      <c r="M5" s="74" t="s">
+        <v>207</v>
+      </c>
+      <c r="N5" s="54">
+        <v>2</v>
+      </c>
+      <c r="P5" s="75" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q5" s="54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="74" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" s="54">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="54">
+        <v>3</v>
+      </c>
+      <c r="G6" s="74" t="s">
+        <v>209</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="J6" s="74" t="s">
+        <v>216</v>
+      </c>
+      <c r="K6" s="54">
+        <v>3</v>
+      </c>
+      <c r="M6" s="74" t="s">
+        <v>125</v>
+      </c>
+      <c r="N6" s="54">
+        <v>3</v>
+      </c>
+      <c r="P6" s="75" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q6" s="54" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="74" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" s="54">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>191</v>
+      </c>
+      <c r="E7" s="54">
+        <v>4</v>
+      </c>
+      <c r="G7" s="74" t="s">
+        <v>210</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="J7" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="K7" s="54">
+        <v>4</v>
+      </c>
+      <c r="M7" s="74" t="s">
+        <v>210</v>
+      </c>
+      <c r="N7" s="54">
+        <v>4</v>
+      </c>
+      <c r="P7" s="75" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q7" s="54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="74" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" s="54">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>192</v>
+      </c>
+      <c r="E8" s="54">
+        <v>5</v>
+      </c>
+      <c r="G8" s="74" t="s">
+        <v>211</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="J8" s="74" t="s">
+        <v>218</v>
+      </c>
+      <c r="K8" s="54">
+        <v>5</v>
+      </c>
+      <c r="M8" s="74" t="s">
+        <v>213</v>
+      </c>
+      <c r="N8" s="54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="74" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" s="54">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>193</v>
+      </c>
+      <c r="E9" s="54">
+        <v>6</v>
+      </c>
+      <c r="G9" s="74" t="s">
+        <v>127</v>
+      </c>
+      <c r="H9">
+        <v>7</v>
+      </c>
+      <c r="J9" s="74" t="s">
+        <v>222</v>
+      </c>
+      <c r="K9" s="54">
+        <v>6</v>
+      </c>
+      <c r="M9" s="74" t="s">
+        <v>212</v>
+      </c>
+      <c r="N9" s="54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="74" t="s">
+        <v>174</v>
+      </c>
+      <c r="B10" s="54">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E10" s="54">
+        <v>7</v>
+      </c>
+      <c r="G10" s="74" t="s">
+        <v>212</v>
+      </c>
+      <c r="H10" s="54">
+        <v>8</v>
+      </c>
+      <c r="J10" s="74" t="s">
+        <v>223</v>
+      </c>
+      <c r="K10" s="54">
+        <v>7</v>
+      </c>
+      <c r="M10" s="74" t="s">
+        <v>124</v>
+      </c>
+      <c r="N10" s="54">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="74" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11" s="54">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>195</v>
+      </c>
+      <c r="E11" s="54">
+        <v>8</v>
+      </c>
+      <c r="G11" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="H11" s="54">
+        <v>9</v>
+      </c>
+      <c r="J11" s="74" t="s">
+        <v>224</v>
+      </c>
+      <c r="K11" s="54">
+        <v>8</v>
+      </c>
+      <c r="M11" s="74" t="s">
+        <v>215</v>
+      </c>
+      <c r="N11" s="54">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="74" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12" s="54">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>196</v>
+      </c>
+      <c r="E12" s="54">
+        <v>9</v>
+      </c>
+      <c r="G12" s="74" t="s">
+        <v>214</v>
+      </c>
+      <c r="H12" s="54">
+        <v>10</v>
+      </c>
+      <c r="J12" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="K12" s="54">
+        <v>9</v>
+      </c>
+      <c r="M12" s="74" t="s">
+        <v>233</v>
+      </c>
+      <c r="N12" s="54">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="74" t="s">
+        <v>177</v>
+      </c>
+      <c r="B13" s="54">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>197</v>
+      </c>
+      <c r="E13" s="54">
+        <v>10</v>
+      </c>
+      <c r="G13" s="74" t="s">
+        <v>215</v>
+      </c>
+      <c r="H13" s="54">
+        <v>12</v>
+      </c>
+      <c r="J13" s="74" t="s">
+        <v>193</v>
+      </c>
+      <c r="K13" s="54">
+        <v>10</v>
+      </c>
+      <c r="M13" s="74" t="s">
+        <v>188</v>
+      </c>
+      <c r="N13" s="54">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="74" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14" s="54">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>198</v>
+      </c>
+      <c r="E14" s="54">
+        <v>11</v>
+      </c>
+      <c r="G14" s="74" t="s">
+        <v>216</v>
+      </c>
+      <c r="H14" s="54">
+        <v>13</v>
+      </c>
+      <c r="J14" s="74" t="s">
+        <v>194</v>
+      </c>
+      <c r="K14" s="54">
+        <v>11</v>
+      </c>
+      <c r="M14" s="74" t="s">
+        <v>218</v>
+      </c>
+      <c r="N14" s="54">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="74" t="s">
+        <v>179</v>
+      </c>
+      <c r="B15" s="54">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>199</v>
+      </c>
+      <c r="E15" s="54">
+        <v>12</v>
+      </c>
+      <c r="G15" s="74" t="s">
+        <v>217</v>
+      </c>
+      <c r="H15" s="54">
+        <v>14</v>
+      </c>
+      <c r="J15" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="K15" s="54">
+        <v>12</v>
+      </c>
+      <c r="M15" s="74" t="s">
+        <v>222</v>
+      </c>
+      <c r="N15" s="54">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="74" t="s">
+        <v>180</v>
+      </c>
+      <c r="B16" s="54">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>200</v>
+      </c>
+      <c r="E16" s="54">
+        <v>13</v>
+      </c>
+      <c r="G16" s="74" t="s">
+        <v>188</v>
+      </c>
+      <c r="H16" s="54">
+        <v>15</v>
+      </c>
+      <c r="J16" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="K16" s="54">
+        <v>13</v>
+      </c>
+      <c r="M16" s="74" t="s">
+        <v>223</v>
+      </c>
+      <c r="N16" s="54">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="74" t="s">
+        <v>181</v>
+      </c>
+      <c r="B17" s="54">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>201</v>
+      </c>
+      <c r="E17" s="54">
+        <v>14</v>
+      </c>
+      <c r="G17" s="74" t="s">
+        <v>218</v>
+      </c>
+      <c r="H17" s="54">
+        <v>16</v>
+      </c>
+      <c r="J17" s="74" t="s">
+        <v>228</v>
+      </c>
+      <c r="K17" s="54">
+        <v>14</v>
+      </c>
+      <c r="M17" s="74" t="s">
+        <v>224</v>
+      </c>
+      <c r="N17" s="54">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="74" t="s">
+        <v>182</v>
+      </c>
+      <c r="B18" s="54">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>202</v>
+      </c>
+      <c r="E18" s="54">
+        <v>15</v>
+      </c>
+      <c r="G18" s="74" t="s">
+        <v>219</v>
+      </c>
+      <c r="H18" s="54">
+        <v>18</v>
+      </c>
+      <c r="J18" s="74" t="s">
+        <v>229</v>
+      </c>
+      <c r="K18" s="54">
+        <v>15</v>
+      </c>
+      <c r="M18" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="N18" s="54">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="74" t="s">
+        <v>183</v>
+      </c>
+      <c r="B19" s="54">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>203</v>
+      </c>
+      <c r="E19" s="54">
+        <v>16</v>
+      </c>
+      <c r="G19" s="74" t="s">
+        <v>190</v>
+      </c>
+      <c r="H19" s="54">
+        <v>19</v>
+      </c>
+      <c r="J19" s="74" t="s">
+        <v>230</v>
+      </c>
+      <c r="K19" s="54">
+        <v>16</v>
+      </c>
+      <c r="M19" s="74" t="s">
+        <v>234</v>
+      </c>
+      <c r="N19" s="54">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="74" t="s">
+        <v>185</v>
+      </c>
+      <c r="B20" s="54">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>204</v>
+      </c>
+      <c r="E20" s="54">
+        <v>17</v>
+      </c>
+      <c r="G20" s="74" t="s">
+        <v>220</v>
+      </c>
+      <c r="H20" s="54">
+        <v>20</v>
+      </c>
+      <c r="J20" s="74" t="s">
+        <v>231</v>
+      </c>
+      <c r="K20" s="54">
+        <v>17</v>
+      </c>
+      <c r="M20" s="74" t="s">
+        <v>235</v>
+      </c>
+      <c r="N20" s="54">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="74" t="s">
+        <v>184</v>
+      </c>
+      <c r="B21" s="54">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>205</v>
+      </c>
+      <c r="E21" s="54">
+        <v>18</v>
+      </c>
+      <c r="J21" s="74" t="s">
+        <v>232</v>
+      </c>
+      <c r="K21" s="54">
+        <v>18</v>
+      </c>
+      <c r="M21" s="74" t="s">
+        <v>195</v>
+      </c>
+      <c r="N21" s="54">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>206</v>
+      </c>
+      <c r="E22" s="54">
+        <v>19</v>
+      </c>
+      <c r="J22" s="74" t="s">
+        <v>201</v>
+      </c>
+      <c r="K22" s="54">
+        <v>19</v>
+      </c>
+      <c r="M22" s="74" t="s">
+        <v>196</v>
+      </c>
+      <c r="N22" s="54">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="54">
+        <v>20</v>
+      </c>
+      <c r="J23" s="74" t="s">
+        <v>202</v>
+      </c>
+      <c r="K23" s="54">
+        <v>20</v>
+      </c>
+      <c r="M23" s="74" t="s">
+        <v>236</v>
+      </c>
+      <c r="N23" s="54">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D15415-B66E-4FEA-A98E-B2D6FD0A9481}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2504,7 +3497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B2F4E0-04ED-4419-995D-BAD7964855D3}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:B7"/>
@@ -2576,7 +3569,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8902D759-323D-4CCA-8BAF-52341B40277A}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:B7"/>
@@ -2648,7 +3641,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{022C6AC2-F769-4CFA-A8C8-9F62F3C69E29}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:B7"/>
@@ -2720,7 +3713,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D471B223-FE94-40E2-BCDA-46194F85E0A6}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:B7"/>
@@ -2788,6 +3781,34 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E603AF88-1493-419E-A47E-525FA0DBED1A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7FC0B5A-8DF3-414E-B3BC-A3DB8B5A2D93}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8574,7 +9595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0AE8A38-5DA2-4530-BB75-4D604A894296}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -9490,8 +10511,8 @@
       <c r="J2" s="62"/>
       <c r="M2" s="59"/>
       <c r="N2" s="59"/>
-      <c r="O2" s="76"/>
-      <c r="P2" s="76"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="77"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="70">
@@ -9509,8 +10530,8 @@
       <c r="J3" s="62"/>
       <c r="M3" s="64"/>
       <c r="N3" s="64"/>
-      <c r="O3" s="76"/>
-      <c r="P3" s="76"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="70">
@@ -9528,8 +10549,8 @@
       <c r="J4" s="62"/>
       <c r="M4" s="64"/>
       <c r="N4" s="64"/>
-      <c r="O4" s="76"/>
-      <c r="P4" s="76"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="70">
@@ -9547,8 +10568,8 @@
       <c r="J5" s="62"/>
       <c r="M5" s="64"/>
       <c r="N5" s="64"/>
-      <c r="O5" s="76"/>
-      <c r="P5" s="76"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="77"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="70">
@@ -9566,8 +10587,8 @@
       <c r="J6" s="62"/>
       <c r="M6" s="64"/>
       <c r="N6" s="64"/>
-      <c r="O6" s="76"/>
-      <c r="P6" s="76"/>
+      <c r="O6" s="77"/>
+      <c r="P6" s="77"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="70">
@@ -9585,8 +10606,8 @@
       <c r="J7" s="62"/>
       <c r="M7" s="64"/>
       <c r="N7" s="64"/>
-      <c r="O7" s="76"/>
-      <c r="P7" s="76"/>
+      <c r="O7" s="77"/>
+      <c r="P7" s="77"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="70">
@@ -9604,8 +10625,8 @@
       <c r="J8" s="62"/>
       <c r="M8" s="64"/>
       <c r="N8" s="64"/>
-      <c r="O8" s="76"/>
-      <c r="P8" s="76"/>
+      <c r="O8" s="77"/>
+      <c r="P8" s="77"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="70">
@@ -9623,8 +10644,8 @@
       <c r="J9" s="62"/>
       <c r="M9" s="64"/>
       <c r="N9" s="64"/>
-      <c r="O9" s="76"/>
-      <c r="P9" s="76"/>
+      <c r="O9" s="77"/>
+      <c r="P9" s="77"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="62"/>
@@ -9636,8 +10657,8 @@
       <c r="J10" s="62"/>
       <c r="M10" s="64"/>
       <c r="N10" s="64"/>
-      <c r="O10" s="76"/>
-      <c r="P10" s="76"/>
+      <c r="O10" s="77"/>
+      <c r="P10" s="77"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="67" t="s">
@@ -9658,8 +10679,8 @@
       <c r="J11" s="62"/>
       <c r="M11" s="64"/>
       <c r="N11" s="64"/>
-      <c r="O11" s="76"/>
-      <c r="P11" s="76"/>
+      <c r="O11" s="77"/>
+      <c r="P11" s="77"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="70">
@@ -9680,8 +10701,8 @@
       <c r="J12" s="62"/>
       <c r="M12" s="64"/>
       <c r="N12" s="64"/>
-      <c r="O12" s="76"/>
-      <c r="P12" s="76"/>
+      <c r="O12" s="77"/>
+      <c r="P12" s="77"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="70">
@@ -9702,8 +10723,8 @@
       <c r="J13" s="62"/>
       <c r="M13" s="64"/>
       <c r="N13" s="61"/>
-      <c r="O13" s="76"/>
-      <c r="P13" s="76"/>
+      <c r="O13" s="77"/>
+      <c r="P13" s="77"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="70">

</xml_diff>

<commit_message>
Add Papi Kostick + Tintum Anak
</commit_message>
<xml_diff>
--- a/backend/src/data/test_norma.xlsx
+++ b/backend/src/data/test_norma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Important Files\Informatika ISTTS\_Semester 6\Kerja_Praktek\Project\adiputro_psytest_backend\backend\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7110767C-18FC-4D9A-8FB6-6B2C60B229AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886FE85A-F869-45A7-8B66-59C3B3388AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="3" activeTab="16" xr2:uid="{28313136-274B-432F-8942-0592E5394583}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="10" activeTab="15" xr2:uid="{28313136-274B-432F-8942-0592E5394583}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="11" r:id="rId1"/>
@@ -28,8 +28,9 @@
     <sheet name="13" sheetId="7" r:id="rId13"/>
     <sheet name="14" sheetId="8" r:id="rId14"/>
     <sheet name="15" sheetId="9" r:id="rId15"/>
-    <sheet name="17" sheetId="16" r:id="rId16"/>
-    <sheet name="21" sheetId="17" r:id="rId17"/>
+    <sheet name="16" sheetId="18" r:id="rId16"/>
+    <sheet name="17" sheetId="16" r:id="rId17"/>
+    <sheet name="21" sheetId="17" r:id="rId18"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="278">
   <si>
     <t>College Student (Men)</t>
   </si>
@@ -775,6 +776,114 @@
   </si>
   <si>
     <t>7-7,9</t>
+  </si>
+  <si>
+    <t>0-0</t>
+  </si>
+  <si>
+    <t>1-1</t>
+  </si>
+  <si>
+    <t>1-3</t>
+  </si>
+  <si>
+    <t>0-3</t>
+  </si>
+  <si>
+    <t>2-2</t>
+  </si>
+  <si>
+    <t>3-3</t>
+  </si>
+  <si>
+    <t>4-4</t>
+  </si>
+  <si>
+    <t>5-6</t>
+  </si>
+  <si>
+    <t>7-8</t>
+  </si>
+  <si>
+    <t>10-11</t>
+  </si>
+  <si>
+    <t>15-19</t>
+  </si>
+  <si>
+    <t>0-13</t>
+  </si>
+  <si>
+    <t>20-21</t>
+  </si>
+  <si>
+    <t>24-25</t>
+  </si>
+  <si>
+    <t>30-32</t>
+  </si>
+  <si>
+    <t>37-38</t>
+  </si>
+  <si>
+    <t>39-40</t>
+  </si>
+  <si>
+    <t>22-22</t>
+  </si>
+  <si>
+    <t>23-23</t>
+  </si>
+  <si>
+    <t>26-26</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>13-15</t>
+  </si>
+  <si>
+    <t>0-18</t>
+  </si>
+  <si>
+    <t>27-28</t>
+  </si>
+  <si>
+    <t>34-35</t>
+  </si>
+  <si>
+    <t>38-38</t>
+  </si>
+  <si>
+    <t>16-18</t>
+  </si>
+  <si>
+    <t>17-18</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>4-5</t>
+  </si>
+  <si>
+    <t>11-12</t>
+  </si>
+  <si>
+    <t>0-12</t>
+  </si>
+  <si>
+    <t>29-29</t>
+  </si>
+  <si>
+    <t>33-33</t>
+  </si>
+  <si>
+    <t>4-7</t>
+  </si>
+  <si>
+    <t>16-19</t>
   </si>
 </sst>
 </file>
@@ -2668,8 +2777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E425E2-BA8B-44FA-A16E-BB1E0B68198A}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B21" sqref="A1:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3786,6 +3895,1383 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80ECB89-F1E8-407D-8EEE-EA36F8B6F8A0}">
+  <dimension ref="A1:Z33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25:E31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="76" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="D1" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="56"/>
+      <c r="G1" s="76" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="56"/>
+      <c r="J1" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="56"/>
+      <c r="M1" s="76" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="56"/>
+      <c r="P1" s="76" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="56"/>
+      <c r="S1" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" s="56"/>
+      <c r="V1" s="76" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" s="56"/>
+      <c r="Y1" s="76" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="56"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="G2" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="J2" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="K2" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="M2" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="N2" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="P2" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q2" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="S2" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="T2" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="V2" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="W2" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y2" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="Z2" s="56" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
+        <v>242</v>
+      </c>
+      <c r="B3" s="54">
+        <v>0</v>
+      </c>
+      <c r="D3" s="74" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3" s="54">
+        <v>0</v>
+      </c>
+      <c r="G3" s="74" t="s">
+        <v>253</v>
+      </c>
+      <c r="H3" s="54">
+        <v>0</v>
+      </c>
+      <c r="J3" s="74" t="s">
+        <v>264</v>
+      </c>
+      <c r="K3" s="54">
+        <v>0</v>
+      </c>
+      <c r="M3" s="74" t="s">
+        <v>244</v>
+      </c>
+      <c r="N3" s="54">
+        <v>0</v>
+      </c>
+      <c r="P3" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q3" s="54">
+        <v>3</v>
+      </c>
+      <c r="S3" s="74" t="s">
+        <v>72</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="V3" s="74" t="s">
+        <v>120</v>
+      </c>
+      <c r="W3" s="54">
+        <v>2</v>
+      </c>
+      <c r="Y3" s="74" t="s">
+        <v>273</v>
+      </c>
+      <c r="Z3" s="54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
+        <v>243</v>
+      </c>
+      <c r="B4" s="54">
+        <v>1</v>
+      </c>
+      <c r="D4" s="74" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="54">
+        <v>1</v>
+      </c>
+      <c r="G4" s="74" t="s">
+        <v>215</v>
+      </c>
+      <c r="H4" s="54">
+        <v>1</v>
+      </c>
+      <c r="J4" s="74" t="s">
+        <v>219</v>
+      </c>
+      <c r="K4" s="54">
+        <v>1</v>
+      </c>
+      <c r="M4" s="74" t="s">
+        <v>248</v>
+      </c>
+      <c r="N4" s="54">
+        <v>1</v>
+      </c>
+      <c r="P4" s="74" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q4" s="54">
+        <v>4</v>
+      </c>
+      <c r="S4" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="T4" s="54">
+        <v>1</v>
+      </c>
+      <c r="V4" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="W4" s="54">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="74" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z4" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="74" t="s">
+        <v>246</v>
+      </c>
+      <c r="B5" s="54">
+        <v>2</v>
+      </c>
+      <c r="D5" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="E5" s="54">
+        <v>2</v>
+      </c>
+      <c r="G5" s="74" t="s">
+        <v>216</v>
+      </c>
+      <c r="H5" s="54">
+        <v>2</v>
+      </c>
+      <c r="J5" s="74" t="s">
+        <v>254</v>
+      </c>
+      <c r="K5" s="54">
+        <v>2</v>
+      </c>
+      <c r="M5" s="74" t="s">
+        <v>207</v>
+      </c>
+      <c r="N5" s="54">
+        <v>3</v>
+      </c>
+      <c r="P5" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q5" s="54">
+        <v>5</v>
+      </c>
+      <c r="S5" s="74" t="s">
+        <v>214</v>
+      </c>
+      <c r="T5" s="54">
+        <v>2</v>
+      </c>
+      <c r="V5" s="74" t="s">
+        <v>249</v>
+      </c>
+      <c r="W5" s="54">
+        <v>4</v>
+      </c>
+      <c r="Y5" s="74" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z5" s="54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="74" t="s">
+        <v>247</v>
+      </c>
+      <c r="B6" s="54">
+        <v>3</v>
+      </c>
+      <c r="D6" s="74" t="s">
+        <v>189</v>
+      </c>
+      <c r="E6" s="54">
+        <v>3</v>
+      </c>
+      <c r="G6" s="74" t="s">
+        <v>217</v>
+      </c>
+      <c r="H6" s="54">
+        <v>3</v>
+      </c>
+      <c r="J6" s="74" t="s">
+        <v>224</v>
+      </c>
+      <c r="K6" s="54">
+        <v>3</v>
+      </c>
+      <c r="M6" s="74" t="s">
+        <v>208</v>
+      </c>
+      <c r="N6" s="54">
+        <v>4</v>
+      </c>
+      <c r="P6" s="74" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q6" s="54">
+        <v>6</v>
+      </c>
+      <c r="S6" s="74" t="s">
+        <v>129</v>
+      </c>
+      <c r="T6" s="54">
+        <v>3</v>
+      </c>
+      <c r="V6" s="74" t="s">
+        <v>250</v>
+      </c>
+      <c r="W6" s="54">
+        <v>5</v>
+      </c>
+      <c r="Y6" s="74" t="s">
+        <v>217</v>
+      </c>
+      <c r="Z6" s="54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="74" t="s">
+        <v>248</v>
+      </c>
+      <c r="B7" s="54">
+        <v>4</v>
+      </c>
+      <c r="D7" s="74" t="s">
+        <v>254</v>
+      </c>
+      <c r="E7" s="54">
+        <v>4</v>
+      </c>
+      <c r="G7" s="74" t="s">
+        <v>188</v>
+      </c>
+      <c r="H7" s="54">
+        <v>4</v>
+      </c>
+      <c r="J7" s="74" t="s">
+        <v>255</v>
+      </c>
+      <c r="K7" s="54">
+        <v>4</v>
+      </c>
+      <c r="M7" s="74" t="s">
+        <v>209</v>
+      </c>
+      <c r="N7" s="54">
+        <v>6</v>
+      </c>
+      <c r="P7" s="74" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q7" s="54">
+        <v>7</v>
+      </c>
+      <c r="S7" s="74" t="s">
+        <v>217</v>
+      </c>
+      <c r="T7" s="54">
+        <v>4</v>
+      </c>
+      <c r="V7" s="74" t="s">
+        <v>211</v>
+      </c>
+      <c r="W7" s="54">
+        <v>6</v>
+      </c>
+      <c r="Y7" s="74" t="s">
+        <v>269</v>
+      </c>
+      <c r="Z7" s="54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="74" t="s">
+        <v>249</v>
+      </c>
+      <c r="B8" s="54">
+        <v>5</v>
+      </c>
+      <c r="D8" s="74" t="s">
+        <v>224</v>
+      </c>
+      <c r="E8" s="54">
+        <v>5</v>
+      </c>
+      <c r="G8" s="74" t="s">
+        <v>218</v>
+      </c>
+      <c r="H8" s="54">
+        <v>5</v>
+      </c>
+      <c r="J8" s="74" t="s">
+        <v>261</v>
+      </c>
+      <c r="K8" s="54">
+        <v>5</v>
+      </c>
+      <c r="M8" s="74" t="s">
+        <v>210</v>
+      </c>
+      <c r="N8" s="54">
+        <v>7</v>
+      </c>
+      <c r="P8" s="74" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q8" s="54">
+        <v>8</v>
+      </c>
+      <c r="S8" s="74" t="s">
+        <v>269</v>
+      </c>
+      <c r="T8" s="54">
+        <v>5</v>
+      </c>
+      <c r="V8" s="74" t="s">
+        <v>251</v>
+      </c>
+      <c r="W8" s="54">
+        <v>7</v>
+      </c>
+      <c r="Y8" s="74" t="s">
+        <v>219</v>
+      </c>
+      <c r="Z8" s="54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="74" t="s">
+        <v>209</v>
+      </c>
+      <c r="B9" s="54">
+        <v>6</v>
+      </c>
+      <c r="D9" s="74" t="s">
+        <v>255</v>
+      </c>
+      <c r="E9" s="54">
+        <v>6</v>
+      </c>
+      <c r="G9" s="74" t="s">
+        <v>219</v>
+      </c>
+      <c r="H9" s="54">
+        <v>6</v>
+      </c>
+      <c r="J9" s="74" t="s">
+        <v>265</v>
+      </c>
+      <c r="K9" s="54">
+        <v>6</v>
+      </c>
+      <c r="M9" s="74" t="s">
+        <v>211</v>
+      </c>
+      <c r="N9" s="54">
+        <v>9</v>
+      </c>
+      <c r="P9" s="74" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q9" s="54">
+        <v>9</v>
+      </c>
+      <c r="S9" s="74" t="s">
+        <v>219</v>
+      </c>
+      <c r="T9" s="54">
+        <v>6</v>
+      </c>
+      <c r="V9" s="74" t="s">
+        <v>124</v>
+      </c>
+      <c r="W9" s="54">
+        <v>8</v>
+      </c>
+      <c r="Y9" s="74" t="s">
+        <v>254</v>
+      </c>
+      <c r="Z9" s="54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="74" t="s">
+        <v>210</v>
+      </c>
+      <c r="B10" s="54">
+        <v>7</v>
+      </c>
+      <c r="D10" s="74" t="s">
+        <v>194</v>
+      </c>
+      <c r="E10" s="54">
+        <v>7</v>
+      </c>
+      <c r="G10" s="74" t="s">
+        <v>254</v>
+      </c>
+      <c r="H10" s="54">
+        <v>7</v>
+      </c>
+      <c r="J10" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="K10" s="54">
+        <v>7</v>
+      </c>
+      <c r="M10" s="74" t="s">
+        <v>127</v>
+      </c>
+      <c r="N10" s="54">
+        <v>10</v>
+      </c>
+      <c r="P10" s="74" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q10" s="54">
+        <v>10</v>
+      </c>
+      <c r="S10" s="74" t="s">
+        <v>254</v>
+      </c>
+      <c r="T10" s="54">
+        <v>7</v>
+      </c>
+      <c r="V10" s="74" t="s">
+        <v>129</v>
+      </c>
+      <c r="W10" s="54">
+        <v>9</v>
+      </c>
+      <c r="Y10" s="74" t="s">
+        <v>259</v>
+      </c>
+      <c r="Z10" s="54">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="74" t="s">
+        <v>211</v>
+      </c>
+      <c r="B11" s="54">
+        <v>8</v>
+      </c>
+      <c r="D11" s="74" t="s">
+        <v>195</v>
+      </c>
+      <c r="E11" s="54">
+        <v>8</v>
+      </c>
+      <c r="G11" s="74" t="s">
+        <v>259</v>
+      </c>
+      <c r="H11" s="54">
+        <v>8</v>
+      </c>
+      <c r="J11" s="74" t="s">
+        <v>228</v>
+      </c>
+      <c r="K11" s="54">
+        <v>8</v>
+      </c>
+      <c r="M11" s="74" t="s">
+        <v>212</v>
+      </c>
+      <c r="N11" s="54">
+        <v>12</v>
+      </c>
+      <c r="P11" s="74" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q11" s="54">
+        <v>11</v>
+      </c>
+      <c r="S11" s="74" t="s">
+        <v>259</v>
+      </c>
+      <c r="T11" s="54">
+        <v>8</v>
+      </c>
+      <c r="V11" s="74" t="s">
+        <v>217</v>
+      </c>
+      <c r="W11" s="54">
+        <v>10</v>
+      </c>
+      <c r="Y11" s="74" t="s">
+        <v>260</v>
+      </c>
+      <c r="Z11" s="54">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="74" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" s="54">
+        <v>9</v>
+      </c>
+      <c r="D12" s="74" t="s">
+        <v>256</v>
+      </c>
+      <c r="E12" s="54">
+        <v>9</v>
+      </c>
+      <c r="G12" s="74" t="s">
+        <v>260</v>
+      </c>
+      <c r="H12" s="54">
+        <v>9</v>
+      </c>
+      <c r="J12" s="74" t="s">
+        <v>229</v>
+      </c>
+      <c r="K12" s="54">
+        <v>9</v>
+      </c>
+      <c r="M12" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="N12" s="54">
+        <v>13</v>
+      </c>
+      <c r="P12" s="74" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q12" s="54">
+        <v>12</v>
+      </c>
+      <c r="S12" s="74" t="s">
+        <v>192</v>
+      </c>
+      <c r="T12" s="54">
+        <v>9</v>
+      </c>
+      <c r="V12" s="74" t="s">
+        <v>269</v>
+      </c>
+      <c r="W12" s="54">
+        <v>11</v>
+      </c>
+      <c r="Y12" s="74" t="s">
+        <v>255</v>
+      </c>
+      <c r="Z12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="74" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" s="54">
+        <v>10</v>
+      </c>
+      <c r="D13" s="74" t="s">
+        <v>198</v>
+      </c>
+      <c r="E13" s="54">
+        <v>10</v>
+      </c>
+      <c r="G13" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="H13" s="54">
+        <v>10</v>
+      </c>
+      <c r="J13" s="74" t="s">
+        <v>266</v>
+      </c>
+      <c r="K13" s="54">
+        <v>10</v>
+      </c>
+      <c r="M13" s="74" t="s">
+        <v>214</v>
+      </c>
+      <c r="N13" s="54">
+        <v>15</v>
+      </c>
+      <c r="P13" s="74" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q13" s="54">
+        <v>13</v>
+      </c>
+      <c r="S13" s="74" t="s">
+        <v>193</v>
+      </c>
+      <c r="T13" s="54">
+        <v>10</v>
+      </c>
+      <c r="V13" s="74" t="s">
+        <v>222</v>
+      </c>
+      <c r="W13" s="54">
+        <v>12</v>
+      </c>
+      <c r="Y13" s="74" t="s">
+        <v>261</v>
+      </c>
+      <c r="Z13" s="54">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" s="54">
+        <v>11</v>
+      </c>
+      <c r="D14" s="74" t="s">
+        <v>231</v>
+      </c>
+      <c r="E14" s="54">
+        <v>11</v>
+      </c>
+      <c r="G14" s="74" t="s">
+        <v>193</v>
+      </c>
+      <c r="H14" s="54">
+        <v>11</v>
+      </c>
+      <c r="J14" s="74" t="s">
+        <v>200</v>
+      </c>
+      <c r="K14" s="54">
+        <v>11</v>
+      </c>
+      <c r="M14" s="74" t="s">
+        <v>215</v>
+      </c>
+      <c r="N14" s="54">
+        <v>16</v>
+      </c>
+      <c r="P14" s="74" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q14" s="54">
+        <v>14</v>
+      </c>
+      <c r="S14" s="74" t="s">
+        <v>194</v>
+      </c>
+      <c r="T14" s="54">
+        <v>11</v>
+      </c>
+      <c r="V14" s="74"/>
+      <c r="W14" s="54"/>
+      <c r="Y14" s="74" t="s">
+        <v>265</v>
+      </c>
+      <c r="Z14" s="54">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="74" t="s">
+        <v>214</v>
+      </c>
+      <c r="B15" s="54">
+        <v>12</v>
+      </c>
+      <c r="D15" s="74" t="s">
+        <v>257</v>
+      </c>
+      <c r="E15" s="54">
+        <v>12</v>
+      </c>
+      <c r="G15" s="74" t="s">
+        <v>261</v>
+      </c>
+      <c r="H15" s="54">
+        <v>12</v>
+      </c>
+      <c r="J15" s="74" t="s">
+        <v>267</v>
+      </c>
+      <c r="K15" s="54">
+        <v>12</v>
+      </c>
+      <c r="M15" s="74" t="s">
+        <v>216</v>
+      </c>
+      <c r="N15" s="54">
+        <v>18</v>
+      </c>
+      <c r="P15" s="74" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q15" s="54">
+        <v>15</v>
+      </c>
+      <c r="S15" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="T15" s="54">
+        <v>12</v>
+      </c>
+      <c r="V15" s="74"/>
+      <c r="W15" s="54"/>
+      <c r="Y15" s="74" t="s">
+        <v>274</v>
+      </c>
+      <c r="Z15" s="54">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="74" t="s">
+        <v>215</v>
+      </c>
+      <c r="B16" s="54">
+        <v>13</v>
+      </c>
+      <c r="D16" s="74" t="s">
+        <v>258</v>
+      </c>
+      <c r="E16" s="54">
+        <v>13</v>
+      </c>
+      <c r="G16" s="74" t="s">
+        <v>235</v>
+      </c>
+      <c r="H16" s="54">
+        <v>13</v>
+      </c>
+      <c r="J16" s="74" t="s">
+        <v>258</v>
+      </c>
+      <c r="K16" s="54">
+        <v>13</v>
+      </c>
+      <c r="M16" s="74"/>
+      <c r="N16" s="54"/>
+      <c r="P16" s="74" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q16" s="54">
+        <v>16</v>
+      </c>
+      <c r="S16" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="T16" s="54">
+        <v>13</v>
+      </c>
+      <c r="V16" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="W16" s="54">
+        <v>5</v>
+      </c>
+      <c r="Y16" s="74" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z16" s="54">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" s="74" t="s">
+        <v>216</v>
+      </c>
+      <c r="B17" s="54">
+        <v>14</v>
+      </c>
+      <c r="D17" s="74"/>
+      <c r="E17" s="54"/>
+      <c r="G17" s="74" t="s">
+        <v>195</v>
+      </c>
+      <c r="H17" s="54">
+        <v>14</v>
+      </c>
+      <c r="J17" s="74"/>
+      <c r="K17" s="54"/>
+      <c r="M17" s="74"/>
+      <c r="N17" s="54"/>
+      <c r="P17" s="74"/>
+      <c r="Q17" s="54"/>
+      <c r="S17" s="74"/>
+      <c r="T17" s="54"/>
+      <c r="V17" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="W17" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y17" s="74" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" s="74" t="s">
+        <v>217</v>
+      </c>
+      <c r="B18" s="54">
+        <v>15</v>
+      </c>
+      <c r="D18" s="74"/>
+      <c r="E18" s="54"/>
+      <c r="G18" s="74" t="s">
+        <v>262</v>
+      </c>
+      <c r="H18" s="54">
+        <v>15</v>
+      </c>
+      <c r="J18" s="74"/>
+      <c r="K18" s="54"/>
+      <c r="M18" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="N18" s="54">
+        <v>5</v>
+      </c>
+      <c r="S18" s="54"/>
+      <c r="T18" s="54"/>
+      <c r="V18" s="74" t="s">
+        <v>270</v>
+      </c>
+      <c r="W18" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y18" s="74" t="s">
+        <v>275</v>
+      </c>
+      <c r="Z18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" s="74" t="s">
+        <v>188</v>
+      </c>
+      <c r="B19" s="54">
+        <v>16</v>
+      </c>
+      <c r="D19" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="54">
+        <v>5</v>
+      </c>
+      <c r="J19" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="K19" s="54">
+        <v>5</v>
+      </c>
+      <c r="M19" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="N19" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="P19" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q19" s="54">
+        <v>5</v>
+      </c>
+      <c r="S19" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="T19" s="54">
+        <v>5</v>
+      </c>
+      <c r="V19" s="75" t="s">
+        <v>271</v>
+      </c>
+      <c r="W19" s="54" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" s="74" t="s">
+        <v>218</v>
+      </c>
+      <c r="B20" s="54">
+        <v>17</v>
+      </c>
+      <c r="D20" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="J20" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="K20" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="M20" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="N20" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="P20" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q20" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="S20" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="T20" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="V20" s="75" t="s">
+        <v>122</v>
+      </c>
+      <c r="W20" s="54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" s="74" t="s">
+        <v>219</v>
+      </c>
+      <c r="B21" s="54">
+        <v>18</v>
+      </c>
+      <c r="D21" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="E21" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" s="54">
+        <v>5</v>
+      </c>
+      <c r="J21" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="K21" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="M21" s="75" t="s">
+        <v>117</v>
+      </c>
+      <c r="N21" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="P21" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q21" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="S21" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="T21" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="V21" s="75" t="s">
+        <v>213</v>
+      </c>
+      <c r="W21" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y21" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z21" s="54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" s="74" t="s">
+        <v>190</v>
+      </c>
+      <c r="B22" s="54">
+        <v>19</v>
+      </c>
+      <c r="D22" s="75" t="s">
+        <v>148</v>
+      </c>
+      <c r="E22" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="J22" s="75" t="s">
+        <v>148</v>
+      </c>
+      <c r="K22" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="M22" s="75" t="s">
+        <v>130</v>
+      </c>
+      <c r="N22" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="P22" s="75" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q22" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="S22" s="75" t="s">
+        <v>148</v>
+      </c>
+      <c r="T22" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="V22" s="74" t="s">
+        <v>272</v>
+      </c>
+      <c r="W22" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y22" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z22" s="56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" s="74"/>
+      <c r="D23" s="75" t="s">
+        <v>149</v>
+      </c>
+      <c r="E23" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="74" t="s">
+        <v>120</v>
+      </c>
+      <c r="H23" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="J23" s="75" t="s">
+        <v>149</v>
+      </c>
+      <c r="K23" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="M23" s="75" t="s">
+        <v>263</v>
+      </c>
+      <c r="N23" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="P23" s="75" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q23" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="S23" s="75" t="s">
+        <v>149</v>
+      </c>
+      <c r="T23" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y23" s="74" t="s">
+        <v>245</v>
+      </c>
+      <c r="Z23" s="54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D24" s="75" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" s="75" t="s">
+        <v>121</v>
+      </c>
+      <c r="H24" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="J24" s="75" t="s">
+        <v>123</v>
+      </c>
+      <c r="K24" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="M24" s="74" t="s">
+        <v>268</v>
+      </c>
+      <c r="N24" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="P24" s="75" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q24" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="S24" s="75" t="s">
+        <v>123</v>
+      </c>
+      <c r="T24" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y24" s="75" t="s">
+        <v>276</v>
+      </c>
+      <c r="Z24" s="54" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="54">
+        <v>5</v>
+      </c>
+      <c r="D25" s="74" t="s">
+        <v>124</v>
+      </c>
+      <c r="E25" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="G25" s="75" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="J25" s="74" t="s">
+        <v>124</v>
+      </c>
+      <c r="K25" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="P25" s="74" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q25" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="S25" s="74" t="s">
+        <v>124</v>
+      </c>
+      <c r="T25" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y25" s="75" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z25" s="54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="75" t="s">
+        <v>144</v>
+      </c>
+      <c r="H26" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y26" s="75" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z26" s="54" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="G27" s="74" t="s">
+        <v>263</v>
+      </c>
+      <c r="H27" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y27" s="74" t="s">
+        <v>277</v>
+      </c>
+      <c r="Z27" s="54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="75" t="s">
+        <v>149</v>
+      </c>
+      <c r="B28" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y28" s="56"/>
+      <c r="Z28" s="56"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="75" t="s">
+        <v>123</v>
+      </c>
+      <c r="B29" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y29" s="74"/>
+      <c r="Z29" s="54"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" s="75" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y30" s="75"/>
+      <c r="Z30" s="54"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" s="74" t="s">
+        <v>252</v>
+      </c>
+      <c r="B31" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y31" s="75"/>
+      <c r="Z31" s="54"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y32" s="75"/>
+      <c r="Z32" s="54"/>
+    </row>
+    <row r="33" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y33" s="74"/>
+      <c r="Z33" s="54"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E603AF88-1493-419E-A47E-525FA0DBED1A}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3799,11 +5285,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7FC0B5A-8DF3-414E-B3BC-A3DB8B5A2D93}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -9595,8 +11081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0AE8A38-5DA2-4530-BB75-4D604A894296}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9679,7 +11165,7 @@
   <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+      <selection activeCell="B9" sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Norma + Database
</commit_message>
<xml_diff>
--- a/backend/src/data/test_norma.xlsx
+++ b/backend/src/data/test_norma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Important Files\Informatika ISTTS\_Semester 6\Kerja_Praktek\Project\adiputro_psytest_backend\backend\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886FE85A-F869-45A7-8B66-59C3B3388AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7C9816-AC5C-44CE-B76E-1DD17914B2B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="10" activeTab="15" xr2:uid="{28313136-274B-432F-8942-0592E5394583}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{28313136-274B-432F-8942-0592E5394583}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="11" r:id="rId1"/>
@@ -1614,8 +1614,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1878,7 +1878,7 @@
         <v>4</v>
       </c>
       <c r="N6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="O6" t="s">
         <v>37</v>
@@ -3898,8 +3898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80ECB89-F1E8-407D-8EEE-EA36F8B6F8A0}">
   <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25:E31"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5290,7 +5290,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finish Akudak Calculation + Fix Tintum Norms
</commit_message>
<xml_diff>
--- a/backend/src/data/test_norma.xlsx
+++ b/backend/src/data/test_norma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Important Files\Informatika ISTTS\_Semester 6\Kerja_Praktek\Project\adiputro_psytest_backend\backend\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7C9816-AC5C-44CE-B76E-1DD17914B2B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E1EA60-5BF3-493F-B682-3301FFF160F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{28313136-274B-432F-8942-0592E5394583}"/>
+    <workbookView xWindow="4275" yWindow="0" windowWidth="15375" windowHeight="7995" activeTab="9" xr2:uid="{28313136-274B-432F-8942-0592E5394583}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="11" r:id="rId1"/>
@@ -571,9 +571,6 @@
     <t>12-15</t>
   </si>
   <si>
-    <t>25-299</t>
-  </si>
-  <si>
     <t>30-33</t>
   </si>
   <si>
@@ -604,9 +601,6 @@
     <t>69-73</t>
   </si>
   <si>
-    <t>78-80</t>
-  </si>
-  <si>
     <t>74-77</t>
   </si>
   <si>
@@ -763,21 +757,9 @@
     <t>31-40</t>
   </si>
   <si>
-    <t>0-4,9</t>
-  </si>
-  <si>
     <t>8-999</t>
   </si>
   <si>
-    <t>5-5,9</t>
-  </si>
-  <si>
-    <t>6-6,9</t>
-  </si>
-  <si>
-    <t>7-7,9</t>
-  </si>
-  <si>
     <t>0-0</t>
   </si>
   <si>
@@ -884,6 +866,24 @@
   </si>
   <si>
     <t>16-19</t>
+  </si>
+  <si>
+    <t>78-150</t>
+  </si>
+  <si>
+    <t>25-29</t>
+  </si>
+  <si>
+    <t>7-7.9</t>
+  </si>
+  <si>
+    <t>6-6.9</t>
+  </si>
+  <si>
+    <t>5-5.9</t>
+  </si>
+  <si>
+    <t>0-4.9</t>
   </si>
 </sst>
 </file>
@@ -1614,8 +1614,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2777,8 +2777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E425E2-BA8B-44FA-A16E-BB1E0B68198A}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B21" sqref="A1:B21"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2793,23 +2793,33 @@
       <c r="A1" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="56"/>
+      <c r="B1" s="56">
+        <v>19</v>
+      </c>
       <c r="D1" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="56"/>
+      <c r="E1" s="56">
+        <v>21</v>
+      </c>
       <c r="G1" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="56"/>
+      <c r="H1" s="56">
+        <v>18</v>
+      </c>
       <c r="J1" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="56"/>
+      <c r="K1" s="56">
+        <v>21</v>
+      </c>
       <c r="M1" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="56"/>
+      <c r="N1" s="56">
+        <v>21</v>
+      </c>
       <c r="P1" s="76" t="s">
         <v>78</v>
       </c>
@@ -2822,31 +2832,31 @@
         <v>168</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D2" s="76" t="s">
         <v>168</v>
       </c>
       <c r="E2" s="56" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G2" s="76" t="s">
         <v>168</v>
       </c>
       <c r="H2" s="56" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J2" s="76" t="s">
         <v>168</v>
       </c>
       <c r="K2" s="56" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M2" s="76" t="s">
         <v>168</v>
       </c>
       <c r="N2" s="56" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="P2" s="76" t="s">
         <v>49</v>
@@ -2863,7 +2873,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -2887,7 +2897,7 @@
         <v>0</v>
       </c>
       <c r="P3" s="75" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="Q3" s="54" t="s">
         <v>37</v>
@@ -2901,13 +2911,13 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E4" s="54">
         <v>1</v>
       </c>
       <c r="G4" s="74" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -2925,7 +2935,7 @@
         <v>1</v>
       </c>
       <c r="P4" s="75" t="s">
-        <v>241</v>
+        <v>274</v>
       </c>
       <c r="Q4" s="54" t="s">
         <v>36</v>
@@ -2939,13 +2949,13 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E5" s="54">
         <v>2</v>
       </c>
       <c r="G5" s="74" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -2957,13 +2967,13 @@
         <v>2</v>
       </c>
       <c r="M5" s="74" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="N5" s="54">
         <v>2</v>
       </c>
       <c r="P5" s="75" t="s">
-        <v>240</v>
+        <v>275</v>
       </c>
       <c r="Q5" s="54" t="s">
         <v>35</v>
@@ -2977,19 +2987,19 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E6" s="54">
         <v>3</v>
       </c>
       <c r="G6" s="74" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H6">
         <v>3</v>
       </c>
       <c r="J6" s="74" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K6" s="54">
         <v>3</v>
@@ -3001,7 +3011,7 @@
         <v>3</v>
       </c>
       <c r="P6" s="75" t="s">
-        <v>239</v>
+        <v>276</v>
       </c>
       <c r="Q6" s="54" t="s">
         <v>34</v>
@@ -3015,31 +3025,31 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E7" s="54">
         <v>4</v>
       </c>
       <c r="G7" s="74" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H7">
         <v>4</v>
       </c>
       <c r="J7" s="74" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K7" s="54">
         <v>4</v>
       </c>
       <c r="M7" s="74" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N7" s="54">
         <v>4</v>
       </c>
       <c r="P7" s="75" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="Q7" s="54" t="s">
         <v>33</v>
@@ -3053,25 +3063,25 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E8" s="54">
         <v>5</v>
       </c>
       <c r="G8" s="74" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H8">
         <v>6</v>
       </c>
       <c r="J8" s="74" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="K8" s="54">
         <v>5</v>
       </c>
       <c r="M8" s="74" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="N8" s="54">
         <v>5</v>
@@ -3079,13 +3089,13 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="74" t="s">
-        <v>173</v>
+        <v>273</v>
       </c>
       <c r="B9" s="54">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E9" s="54">
         <v>6</v>
@@ -3097,13 +3107,13 @@
         <v>7</v>
       </c>
       <c r="J9" s="74" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="K9" s="54">
         <v>6</v>
       </c>
       <c r="M9" s="74" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="N9" s="54">
         <v>6</v>
@@ -3111,25 +3121,25 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="74" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B10" s="54">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E10" s="54">
         <v>7</v>
       </c>
       <c r="G10" s="74" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H10" s="54">
         <v>8</v>
       </c>
       <c r="J10" s="74" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="K10" s="54">
         <v>7</v>
@@ -3143,13 +3153,13 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="74" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B11" s="54">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E11" s="54">
         <v>8</v>
@@ -3161,13 +3171,13 @@
         <v>9</v>
       </c>
       <c r="J11" s="74" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="K11" s="54">
         <v>8</v>
       </c>
       <c r="M11" s="74" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="N11" s="54">
         <v>8</v>
@@ -3175,31 +3185,31 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B12" s="54">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E12" s="54">
         <v>9</v>
       </c>
       <c r="G12" s="74" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H12" s="54">
         <v>10</v>
       </c>
       <c r="J12" s="74" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="K12" s="54">
         <v>9</v>
       </c>
       <c r="M12" s="74" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="N12" s="54">
         <v>9</v>
@@ -3207,31 +3217,31 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B13" s="54">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E13" s="54">
         <v>10</v>
       </c>
       <c r="G13" s="74" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H13" s="54">
         <v>12</v>
       </c>
       <c r="J13" s="74" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K13" s="54">
         <v>10</v>
       </c>
       <c r="M13" s="74" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="N13" s="54">
         <v>10</v>
@@ -3239,31 +3249,31 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="74" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B14" s="54">
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E14" s="54">
         <v>11</v>
       </c>
       <c r="G14" s="74" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H14" s="54">
         <v>13</v>
       </c>
       <c r="J14" s="74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K14" s="54">
         <v>11</v>
       </c>
       <c r="M14" s="74" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N14" s="54">
         <v>11</v>
@@ -3271,31 +3281,31 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="74" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B15" s="54">
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E15" s="54">
         <v>12</v>
       </c>
       <c r="G15" s="74" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H15" s="54">
         <v>14</v>
       </c>
       <c r="J15" s="74" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K15" s="54">
         <v>12</v>
       </c>
       <c r="M15" s="74" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N15" s="54">
         <v>12</v>
@@ -3303,31 +3313,31 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="74" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B16" s="54">
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E16" s="54">
         <v>13</v>
       </c>
       <c r="G16" s="74" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H16" s="54">
         <v>15</v>
       </c>
       <c r="J16" s="74" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="K16" s="54">
         <v>13</v>
       </c>
       <c r="M16" s="74" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="N16" s="54">
         <v>13</v>
@@ -3335,31 +3345,31 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="74" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B17" s="54">
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E17" s="54">
         <v>14</v>
       </c>
       <c r="G17" s="74" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H17" s="54">
         <v>16</v>
       </c>
       <c r="J17" s="74" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K17" s="54">
         <v>14</v>
       </c>
       <c r="M17" s="74" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="N17" s="54">
         <v>14</v>
@@ -3367,31 +3377,31 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="74" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B18" s="54">
         <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E18" s="54">
         <v>15</v>
       </c>
       <c r="G18" s="74" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H18" s="54">
         <v>18</v>
       </c>
       <c r="J18" s="74" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K18" s="54">
         <v>15</v>
       </c>
       <c r="M18" s="74" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="N18" s="54">
         <v>15</v>
@@ -3399,31 +3409,31 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="74" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B19" s="54">
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E19" s="54">
         <v>16</v>
       </c>
       <c r="G19" s="74" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H19" s="54">
         <v>19</v>
       </c>
       <c r="J19" s="74" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K19" s="54">
         <v>16</v>
       </c>
       <c r="M19" s="74" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="N19" s="54">
         <v>16</v>
@@ -3431,31 +3441,31 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="74" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B20" s="54">
         <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E20" s="54">
         <v>17</v>
       </c>
       <c r="G20" s="74" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H20" s="54">
         <v>20</v>
       </c>
       <c r="J20" s="74" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K20" s="54">
         <v>17</v>
       </c>
       <c r="M20" s="74" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="N20" s="54">
         <v>17</v>
@@ -3463,25 +3473,25 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="74" t="s">
-        <v>184</v>
+        <v>272</v>
       </c>
       <c r="B21" s="54">
         <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E21" s="54">
         <v>18</v>
       </c>
       <c r="J21" s="74" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K21" s="54">
         <v>18</v>
       </c>
       <c r="M21" s="74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="N21" s="54">
         <v>18</v>
@@ -3489,19 +3499,19 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E22" s="54">
         <v>19</v>
       </c>
       <c r="J22" s="74" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="K22" s="54">
         <v>19</v>
       </c>
       <c r="M22" s="74" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="N22" s="54">
         <v>19</v>
@@ -3515,13 +3525,13 @@
         <v>20</v>
       </c>
       <c r="J23" s="74" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K23" s="54">
         <v>20</v>
       </c>
       <c r="M23" s="74" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="N23" s="54">
         <v>20</v>
@@ -3947,84 +3957,84 @@
         <v>168</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D2" s="76" t="s">
         <v>168</v>
       </c>
       <c r="E2" s="56" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G2" s="76" t="s">
         <v>168</v>
       </c>
       <c r="H2" s="56" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J2" s="76" t="s">
         <v>168</v>
       </c>
       <c r="K2" s="56" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M2" s="76" t="s">
         <v>168</v>
       </c>
       <c r="N2" s="56" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="P2" s="76" t="s">
         <v>168</v>
       </c>
       <c r="Q2" s="56" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="S2" s="76" t="s">
         <v>168</v>
       </c>
       <c r="T2" s="56" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="V2" s="76" t="s">
         <v>168</v>
       </c>
       <c r="W2" s="56" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="Y2" s="76" t="s">
         <v>168</v>
       </c>
       <c r="Z2" s="56" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="74" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B3" s="54">
         <v>0</v>
       </c>
       <c r="D3" s="74" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="E3" s="54">
         <v>0</v>
       </c>
       <c r="G3" s="74" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="H3" s="54">
         <v>0</v>
       </c>
       <c r="J3" s="74" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="K3" s="54">
         <v>0</v>
       </c>
       <c r="M3" s="74" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="N3" s="54">
         <v>0</v>
@@ -4048,7 +4058,7 @@
         <v>2</v>
       </c>
       <c r="Y3" s="74" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="Z3" s="54">
         <v>0</v>
@@ -4056,7 +4066,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="74" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B4" s="54">
         <v>1</v>
@@ -4068,25 +4078,25 @@
         <v>1</v>
       </c>
       <c r="G4" s="74" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H4" s="54">
         <v>1</v>
       </c>
       <c r="J4" s="74" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K4" s="54">
         <v>1</v>
       </c>
       <c r="M4" s="74" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="N4" s="54">
         <v>1</v>
       </c>
       <c r="P4" s="74" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="Q4" s="54">
         <v>4</v>
@@ -4112,31 +4122,31 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="74" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B5" s="54">
         <v>2</v>
       </c>
       <c r="D5" s="74" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E5" s="54">
         <v>2</v>
       </c>
       <c r="G5" s="74" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H5" s="54">
         <v>2</v>
       </c>
       <c r="J5" s="74" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="K5" s="54">
         <v>2</v>
       </c>
       <c r="M5" s="74" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="N5" s="54">
         <v>3</v>
@@ -4148,19 +4158,19 @@
         <v>5</v>
       </c>
       <c r="S5" s="74" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="T5" s="54">
         <v>2</v>
       </c>
       <c r="V5" s="74" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="W5" s="54">
         <v>4</v>
       </c>
       <c r="Y5" s="74" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="Z5" s="54">
         <v>2</v>
@@ -4168,37 +4178,37 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="74" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B6" s="54">
         <v>3</v>
       </c>
       <c r="D6" s="74" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E6" s="54">
         <v>3</v>
       </c>
       <c r="G6" s="74" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H6" s="54">
         <v>3</v>
       </c>
       <c r="J6" s="74" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="K6" s="54">
         <v>3</v>
       </c>
       <c r="M6" s="74" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="N6" s="54">
         <v>4</v>
       </c>
       <c r="P6" s="74" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="Q6" s="54">
         <v>6</v>
@@ -4210,13 +4220,13 @@
         <v>3</v>
       </c>
       <c r="V6" s="74" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="W6" s="54">
         <v>5</v>
       </c>
       <c r="Y6" s="74" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="Z6" s="54">
         <v>3</v>
@@ -4224,31 +4234,31 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="74" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B7" s="54">
         <v>4</v>
       </c>
       <c r="D7" s="74" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="E7" s="54">
         <v>4</v>
       </c>
       <c r="G7" s="74" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H7" s="54">
         <v>4</v>
       </c>
       <c r="J7" s="74" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="K7" s="54">
         <v>4</v>
       </c>
       <c r="M7" s="74" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="N7" s="54">
         <v>6</v>
@@ -4260,19 +4270,19 @@
         <v>7</v>
       </c>
       <c r="S7" s="74" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="T7" s="54">
         <v>4</v>
       </c>
       <c r="V7" s="74" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="W7" s="54">
         <v>6</v>
       </c>
       <c r="Y7" s="74" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="Z7" s="54">
         <v>4</v>
@@ -4280,55 +4290,55 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="74" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B8" s="54">
         <v>5</v>
       </c>
       <c r="D8" s="74" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E8" s="54">
         <v>5</v>
       </c>
       <c r="G8" s="74" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H8" s="54">
         <v>5</v>
       </c>
       <c r="J8" s="74" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="K8" s="54">
         <v>5</v>
       </c>
       <c r="M8" s="74" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N8" s="54">
         <v>7</v>
       </c>
       <c r="P8" s="74" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="Q8" s="54">
         <v>8</v>
       </c>
       <c r="S8" s="74" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="T8" s="54">
         <v>5</v>
       </c>
       <c r="V8" s="74" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="W8" s="54">
         <v>7</v>
       </c>
       <c r="Y8" s="74" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="Z8" s="54">
         <v>5</v>
@@ -4336,43 +4346,43 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="74" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B9" s="54">
         <v>6</v>
       </c>
       <c r="D9" s="74" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="E9" s="54">
         <v>6</v>
       </c>
       <c r="G9" s="74" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H9" s="54">
         <v>6</v>
       </c>
       <c r="J9" s="74" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="K9" s="54">
         <v>6</v>
       </c>
       <c r="M9" s="74" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="N9" s="54">
         <v>9</v>
       </c>
       <c r="P9" s="74" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="Q9" s="54">
         <v>9</v>
       </c>
       <c r="S9" s="74" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="T9" s="54">
         <v>6</v>
@@ -4384,7 +4394,7 @@
         <v>8</v>
       </c>
       <c r="Y9" s="74" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="Z9" s="54">
         <v>6</v>
@@ -4392,25 +4402,25 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="74" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B10" s="54">
         <v>7</v>
       </c>
       <c r="D10" s="74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E10" s="54">
         <v>7</v>
       </c>
       <c r="G10" s="74" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="H10" s="54">
         <v>7</v>
       </c>
       <c r="J10" s="74" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="K10" s="54">
         <v>7</v>
@@ -4422,13 +4432,13 @@
         <v>10</v>
       </c>
       <c r="P10" s="74" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="Q10" s="54">
         <v>10</v>
       </c>
       <c r="S10" s="74" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="T10" s="54">
         <v>7</v>
@@ -4440,7 +4450,7 @@
         <v>9</v>
       </c>
       <c r="Y10" s="74" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="Z10" s="54">
         <v>7</v>
@@ -4448,31 +4458,31 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="74" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B11" s="54">
         <v>8</v>
       </c>
       <c r="D11" s="74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E11" s="54">
         <v>8</v>
       </c>
       <c r="G11" s="74" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="H11" s="54">
         <v>8</v>
       </c>
       <c r="J11" s="74" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K11" s="54">
         <v>8</v>
       </c>
       <c r="M11" s="74" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="N11" s="54">
         <v>12</v>
@@ -4484,19 +4494,19 @@
         <v>11</v>
       </c>
       <c r="S11" s="74" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="T11" s="54">
         <v>8</v>
       </c>
       <c r="V11" s="74" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="W11" s="54">
         <v>10</v>
       </c>
       <c r="Y11" s="74" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="Z11" s="54">
         <v>8</v>
@@ -4510,19 +4520,19 @@
         <v>9</v>
       </c>
       <c r="D12" s="74" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E12" s="54">
         <v>9</v>
       </c>
       <c r="G12" s="74" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H12" s="54">
         <v>9</v>
       </c>
       <c r="J12" s="74" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K12" s="54">
         <v>9</v>
@@ -4534,25 +4544,25 @@
         <v>13</v>
       </c>
       <c r="P12" s="74" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="Q12" s="54">
         <v>12</v>
       </c>
       <c r="S12" s="74" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="T12" s="54">
         <v>9</v>
       </c>
       <c r="V12" s="74" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="W12" s="54">
         <v>11</v>
       </c>
       <c r="Y12" s="74" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="Z12">
         <v>9</v>
@@ -4560,55 +4570,55 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="74" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B13" s="54">
         <v>10</v>
       </c>
       <c r="D13" s="74" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E13" s="54">
         <v>10</v>
       </c>
       <c r="G13" s="74" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H13" s="54">
         <v>10</v>
       </c>
       <c r="J13" s="74" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="K13" s="54">
         <v>10</v>
       </c>
       <c r="M13" s="74" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="N13" s="54">
         <v>15</v>
       </c>
       <c r="P13" s="74" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="Q13" s="54">
         <v>13</v>
       </c>
       <c r="S13" s="74" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="T13" s="54">
         <v>10</v>
       </c>
       <c r="V13" s="74" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="W13" s="54">
         <v>12</v>
       </c>
       <c r="Y13" s="74" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="Z13" s="54">
         <v>10</v>
@@ -4622,37 +4632,37 @@
         <v>11</v>
       </c>
       <c r="D14" s="74" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E14" s="54">
         <v>11</v>
       </c>
       <c r="G14" s="74" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H14" s="54">
         <v>11</v>
       </c>
       <c r="J14" s="74" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K14" s="54">
         <v>11</v>
       </c>
       <c r="M14" s="74" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="N14" s="54">
         <v>16</v>
       </c>
       <c r="P14" s="74" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="Q14" s="54">
         <v>14</v>
       </c>
       <c r="S14" s="74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="T14" s="54">
         <v>11</v>
@@ -4660,7 +4670,7 @@
       <c r="V14" s="74"/>
       <c r="W14" s="54"/>
       <c r="Y14" s="74" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="Z14" s="54">
         <v>11</v>
@@ -4668,43 +4678,43 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="74" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B15" s="54">
         <v>12</v>
       </c>
       <c r="D15" s="74" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="E15" s="54">
         <v>12</v>
       </c>
       <c r="G15" s="74" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="H15" s="54">
         <v>12</v>
       </c>
       <c r="J15" s="74" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="K15" s="54">
         <v>12</v>
       </c>
       <c r="M15" s="74" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="N15" s="54">
         <v>18</v>
       </c>
       <c r="P15" s="74" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="Q15" s="54">
         <v>15</v>
       </c>
       <c r="S15" s="74" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="T15" s="54">
         <v>12</v>
@@ -4712,7 +4722,7 @@
       <c r="V15" s="74"/>
       <c r="W15" s="54"/>
       <c r="Y15" s="74" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="Z15" s="54">
         <v>12</v>
@@ -4720,25 +4730,25 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="74" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B16" s="54">
         <v>13</v>
       </c>
       <c r="D16" s="74" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E16" s="54">
         <v>13</v>
       </c>
       <c r="G16" s="74" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H16" s="54">
         <v>13</v>
       </c>
       <c r="J16" s="74" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="K16" s="54">
         <v>13</v>
@@ -4746,13 +4756,13 @@
       <c r="M16" s="74"/>
       <c r="N16" s="54"/>
       <c r="P16" s="74" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="Q16" s="54">
         <v>16</v>
       </c>
       <c r="S16" s="74" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="T16" s="54">
         <v>13</v>
@@ -4764,7 +4774,7 @@
         <v>5</v>
       </c>
       <c r="Y16" s="74" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="Z16" s="54">
         <v>13</v>
@@ -4772,7 +4782,7 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="74" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B17" s="54">
         <v>14</v>
@@ -4780,7 +4790,7 @@
       <c r="D17" s="74"/>
       <c r="E17" s="54"/>
       <c r="G17" s="74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H17" s="54">
         <v>14</v>
@@ -4800,7 +4810,7 @@
         <v>55</v>
       </c>
       <c r="Y17" s="74" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="Z17">
         <v>14</v>
@@ -4808,7 +4818,7 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="74" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B18" s="54">
         <v>15</v>
@@ -4816,7 +4826,7 @@
       <c r="D18" s="74"/>
       <c r="E18" s="54"/>
       <c r="G18" s="74" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="H18" s="54">
         <v>15</v>
@@ -4832,13 +4842,13 @@
       <c r="S18" s="54"/>
       <c r="T18" s="54"/>
       <c r="V18" s="74" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="W18" s="54" t="s">
         <v>33</v>
       </c>
       <c r="Y18" s="74" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="Z18">
         <v>15</v>
@@ -4846,7 +4856,7 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="74" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B19" s="54">
         <v>16</v>
@@ -4882,7 +4892,7 @@
         <v>5</v>
       </c>
       <c r="V19" s="75" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="W19" s="54" t="s">
         <v>34</v>
@@ -4890,7 +4900,7 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="74" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B20" s="54">
         <v>17</v>
@@ -4934,7 +4944,7 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="74" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B21" s="54">
         <v>18</v>
@@ -4976,7 +4986,7 @@
         <v>33</v>
       </c>
       <c r="V21" s="75" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="W21" s="54" t="s">
         <v>36</v>
@@ -4990,7 +5000,7 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="74" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B22" s="54">
         <v>19</v>
@@ -5032,7 +5042,7 @@
         <v>34</v>
       </c>
       <c r="V22" s="74" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="W22" s="54" t="s">
         <v>37</v>
@@ -5065,7 +5075,7 @@
         <v>35</v>
       </c>
       <c r="M23" s="75" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="N23" s="54" t="s">
         <v>36</v>
@@ -5083,7 +5093,7 @@
         <v>35</v>
       </c>
       <c r="Y23" s="74" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="Z23" s="54" t="s">
         <v>33</v>
@@ -5109,7 +5119,7 @@
         <v>36</v>
       </c>
       <c r="M24" s="74" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="N24" s="54" t="s">
         <v>37</v>
@@ -5127,7 +5137,7 @@
         <v>36</v>
       </c>
       <c r="Y24" s="75" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="Z24" s="54" t="s">
         <v>34</v>
@@ -5159,7 +5169,7 @@
         <v>37</v>
       </c>
       <c r="P25" s="74" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="Q25" s="54" t="s">
         <v>37</v>
@@ -5205,13 +5215,13 @@
         <v>33</v>
       </c>
       <c r="G27" s="74" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="H27" s="54" t="s">
         <v>37</v>
       </c>
       <c r="Y27" s="74" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="Z27" s="54" t="s">
         <v>37</v>
@@ -5249,7 +5259,7 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="74" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B31" s="54" t="s">
         <v>37</v>
@@ -11081,7 +11091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0AE8A38-5DA2-4530-BB75-4D604A894296}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
@@ -11165,7 +11175,7 @@
   <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="A1:B9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finish Tintum Anak Calculation
</commit_message>
<xml_diff>
--- a/backend/src/data/test_norma.xlsx
+++ b/backend/src/data/test_norma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Important Files\Informatika ISTTS\_Semester 6\Kerja_Praktek\Project\adiputro_psytest_backend\backend\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E1EA60-5BF3-493F-B682-3301FFF160F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4872067-B4E0-4C54-9DEE-4149461CD241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="0" windowWidth="15375" windowHeight="7995" activeTab="9" xr2:uid="{28313136-274B-432F-8942-0592E5394583}"/>
+    <workbookView xWindow="4275" yWindow="0" windowWidth="15375" windowHeight="7995" activeTab="15" xr2:uid="{28313136-274B-432F-8942-0592E5394583}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="11" r:id="rId1"/>
@@ -2777,7 +2777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E425E2-BA8B-44FA-A16E-BB1E0B68198A}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
@@ -3908,8 +3908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80ECB89-F1E8-407D-8EEE-EA36F8B6F8A0}">
   <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3918,39 +3918,57 @@
       <c r="A1" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="56"/>
+      <c r="B1" s="56">
+        <v>20</v>
+      </c>
       <c r="D1" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="56"/>
+      <c r="E1" s="56">
+        <v>14</v>
+      </c>
       <c r="G1" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="56"/>
+      <c r="H1" s="56">
+        <v>16</v>
+      </c>
       <c r="J1" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="56"/>
+      <c r="K1" s="56">
+        <v>14</v>
+      </c>
       <c r="M1" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="56"/>
+      <c r="N1" s="56">
+        <v>13</v>
+      </c>
       <c r="P1" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="56"/>
+      <c r="Q1" s="56">
+        <v>14</v>
+      </c>
       <c r="S1" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="56"/>
+      <c r="T1" s="56">
+        <v>14</v>
+      </c>
       <c r="V1" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="W1" s="56"/>
+      <c r="W1" s="56">
+        <v>11</v>
+      </c>
       <c r="Y1" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="56"/>
+      <c r="Z1" s="56">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">

</xml_diff>

<commit_message>
fix minor bug on test_norma.xlsx (tintum anak)
</commit_message>
<xml_diff>
--- a/backend/src/data/test_norma.xlsx
+++ b/backend/src/data/test_norma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\adiputro_psytest_backend\backend\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\adiputro\backend\backend\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B1D80C-EBBE-4CCB-867E-08D64D6501D3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8A941B-75CF-4C03-90A2-3A4DBC173B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4272" yWindow="0" windowWidth="15372" windowHeight="7992" activeTab="15" xr2:uid="{28313136-274B-432F-8942-0592E5394583}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="15" xr2:uid="{28313136-274B-432F-8942-0592E5394583}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="11" r:id="rId1"/>
@@ -32,17 +32,25 @@
     <sheet name="17" sheetId="16" r:id="rId17"/>
     <sheet name="21" sheetId="17" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="278">
   <si>
     <t>College Student (Men)</t>
   </si>
@@ -809,9 +817,6 @@
     <t>26-26</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>13-15</t>
   </si>
   <si>
@@ -873,6 +878,12 @@
   </si>
   <si>
     <t>0-4.9</t>
+  </si>
+  <si>
+    <t>38-40</t>
+  </si>
+  <si>
+    <t>36-36</t>
   </si>
 </sst>
 </file>
@@ -1607,9 +1618,9 @@
       <selection activeCell="B25" sqref="B25:M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" s="20" t="s">
         <v>21</v>
       </c>
@@ -1647,7 +1658,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="20">
         <v>0</v>
       </c>
@@ -1688,7 +1699,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -1732,7 +1743,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <f>A3+1</f>
         <v>2</v>
@@ -1781,7 +1792,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <f t="shared" ref="A5:A22" si="0">A4+1</f>
         <v>3</v>
@@ -1827,7 +1838,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1879,7 +1890,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1925,7 +1936,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1971,7 +1982,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2017,7 +2028,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2063,7 +2074,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2109,7 +2120,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2155,7 +2166,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2198,7 +2209,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2244,7 +2255,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2284,7 +2295,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2324,7 +2335,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2364,7 +2375,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2404,7 +2415,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2444,7 +2455,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
         <f>A19+1</f>
         <v>18</v>
@@ -2481,7 +2492,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2518,7 +2529,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2550,7 +2561,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -2594,7 +2605,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
         <v>41</v>
       </c>
@@ -2629,7 +2640,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -2686,7 +2697,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -2735,13 +2746,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="23"/>
       <c r="B29" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -2749,7 +2760,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -2770,15 +2781,15 @@
       <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="74"/>
-    <col min="7" max="7" width="9.109375" style="74"/>
-    <col min="10" max="10" width="9.109375" style="74"/>
-    <col min="13" max="13" width="9.109375" style="74"/>
+    <col min="1" max="1" width="9.140625" style="74"/>
+    <col min="7" max="7" width="9.140625" style="74"/>
+    <col min="10" max="10" width="9.140625" style="74"/>
+    <col min="13" max="13" width="9.140625" style="74"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="76" t="s">
         <v>21</v>
       </c>
@@ -2816,7 +2827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
         <v>168</v>
       </c>
@@ -2854,7 +2865,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="74" t="s">
         <v>120</v>
       </c>
@@ -2892,7 +2903,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="74" t="s">
         <v>171</v>
       </c>
@@ -2924,13 +2935,13 @@
         <v>1</v>
       </c>
       <c r="P4" s="75" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Q4" s="54" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="74" t="s">
         <v>56</v>
       </c>
@@ -2962,13 +2973,13 @@
         <v>2</v>
       </c>
       <c r="P5" s="75" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Q5" s="54" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="74" t="s">
         <v>172</v>
       </c>
@@ -3000,13 +3011,13 @@
         <v>3</v>
       </c>
       <c r="P6" s="75" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="Q6" s="54" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="74" t="s">
         <v>169</v>
       </c>
@@ -3038,13 +3049,13 @@
         <v>4</v>
       </c>
       <c r="P7" s="75" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="Q7" s="54" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="74" t="s">
         <v>170</v>
       </c>
@@ -3076,9 +3087,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="74" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B9" s="54">
         <v>6</v>
@@ -3108,7 +3119,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="74" t="s">
         <v>173</v>
       </c>
@@ -3140,7 +3151,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="74" t="s">
         <v>174</v>
       </c>
@@ -3172,7 +3183,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
         <v>175</v>
       </c>
@@ -3204,7 +3215,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="74" t="s">
         <v>176</v>
       </c>
@@ -3236,7 +3247,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="74" t="s">
         <v>177</v>
       </c>
@@ -3268,7 +3279,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="74" t="s">
         <v>178</v>
       </c>
@@ -3300,7 +3311,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="74" t="s">
         <v>179</v>
       </c>
@@ -3332,7 +3343,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="74" t="s">
         <v>180</v>
       </c>
@@ -3364,7 +3375,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="74" t="s">
         <v>181</v>
       </c>
@@ -3396,7 +3407,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="74" t="s">
         <v>182</v>
       </c>
@@ -3428,7 +3439,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="74" t="s">
         <v>183</v>
       </c>
@@ -3460,9 +3471,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="74" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B21" s="54">
         <v>18</v>
@@ -3486,7 +3497,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>204</v>
       </c>
@@ -3506,7 +3517,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>59</v>
       </c>
@@ -3542,9 +3553,9 @@
       <selection activeCell="B7" sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>78</v>
       </c>
@@ -3552,7 +3563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>49</v>
       </c>
@@ -3560,7 +3571,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
         <v>68</v>
       </c>
@@ -3568,7 +3579,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
         <v>51</v>
       </c>
@@ -3576,7 +3587,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
         <v>52</v>
       </c>
@@ -3584,7 +3595,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="55" t="s">
         <v>53</v>
       </c>
@@ -3592,7 +3603,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="57" t="s">
         <v>54</v>
       </c>
@@ -3614,9 +3625,9 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>78</v>
       </c>
@@ -3624,7 +3635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
         <v>49</v>
       </c>
@@ -3632,7 +3643,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="45" t="s">
         <v>69</v>
       </c>
@@ -3640,7 +3651,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
         <v>70</v>
       </c>
@@ -3648,7 +3659,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
         <v>81</v>
       </c>
@@ -3656,7 +3667,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
         <v>71</v>
       </c>
@@ -3664,7 +3675,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="45" t="s">
         <v>72</v>
       </c>
@@ -3686,9 +3697,9 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>78</v>
       </c>
@@ -3696,7 +3707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>49</v>
       </c>
@@ -3704,7 +3715,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
         <v>68</v>
       </c>
@@ -3712,7 +3723,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>51</v>
       </c>
@@ -3720,7 +3731,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
         <v>52</v>
       </c>
@@ -3728,7 +3739,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
         <v>53</v>
       </c>
@@ -3736,7 +3747,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="49" t="s">
         <v>54</v>
       </c>
@@ -3758,9 +3769,9 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>78</v>
       </c>
@@ -3768,7 +3779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
         <v>49</v>
       </c>
@@ -3776,7 +3787,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="50" t="s">
         <v>73</v>
       </c>
@@ -3784,7 +3795,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>74</v>
       </c>
@@ -3792,7 +3803,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="53" t="s">
         <v>75</v>
       </c>
@@ -3800,7 +3811,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
         <v>76</v>
       </c>
@@ -3808,7 +3819,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="50" t="s">
         <v>77</v>
       </c>
@@ -3830,9 +3841,9 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>78</v>
       </c>
@@ -3840,7 +3851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
         <v>49</v>
       </c>
@@ -3848,7 +3859,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
         <v>73</v>
       </c>
@@ -3856,7 +3867,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="55" t="s">
         <v>74</v>
       </c>
@@ -3864,7 +3875,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
         <v>75</v>
       </c>
@@ -3872,7 +3883,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="55" t="s">
         <v>76</v>
       </c>
@@ -3880,7 +3891,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="54" t="s">
         <v>77</v>
       </c>
@@ -3898,12 +3909,12 @@
   <dimension ref="A1:Z33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="AG13" sqref="AG13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="76" t="s">
         <v>21</v>
       </c>
@@ -3956,10 +3967,10 @@
         <v>29</v>
       </c>
       <c r="Z1" s="56">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
         <v>168</v>
       </c>
@@ -4015,7 +4026,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="74" t="s">
         <v>236</v>
       </c>
@@ -4035,7 +4046,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="74" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K3" s="54">
         <v>0</v>
@@ -4065,13 +4076,13 @@
         <v>2</v>
       </c>
       <c r="Y3" s="74" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="Z3" s="54">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="74" t="s">
         <v>237</v>
       </c>
@@ -4127,7 +4138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="74" t="s">
         <v>239</v>
       </c>
@@ -4183,7 +4194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="74" t="s">
         <v>240</v>
       </c>
@@ -4239,7 +4250,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="74" t="s">
         <v>241</v>
       </c>
@@ -4289,13 +4300,13 @@
         <v>6</v>
       </c>
       <c r="Y7" s="74" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Z7" s="54">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="74" t="s">
         <v>242</v>
       </c>
@@ -4333,7 +4344,7 @@
         <v>8</v>
       </c>
       <c r="S8" s="74" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="T8" s="54">
         <v>5</v>
@@ -4351,7 +4362,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="74" t="s">
         <v>207</v>
       </c>
@@ -4371,7 +4382,7 @@
         <v>6</v>
       </c>
       <c r="J9" s="74" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K9" s="54">
         <v>6</v>
@@ -4407,7 +4418,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="74" t="s">
         <v>208</v>
       </c>
@@ -4463,7 +4474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="74" t="s">
         <v>209</v>
       </c>
@@ -4519,7 +4530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="74" t="s">
         <v>127</v>
       </c>
@@ -4563,7 +4574,7 @@
         <v>9</v>
       </c>
       <c r="V12" s="74" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="W12" s="54">
         <v>11</v>
@@ -4575,7 +4586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="74" t="s">
         <v>210</v>
       </c>
@@ -4595,7 +4606,7 @@
         <v>10</v>
       </c>
       <c r="J13" s="74" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K13" s="54">
         <v>10</v>
@@ -4631,7 +4642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="74" t="s">
         <v>119</v>
       </c>
@@ -4677,13 +4688,13 @@
       <c r="V14" s="74"/>
       <c r="W14" s="54"/>
       <c r="Y14" s="74" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Z14" s="54">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="74" t="s">
         <v>212</v>
       </c>
@@ -4703,7 +4714,7 @@
         <v>12</v>
       </c>
       <c r="J15" s="74" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K15" s="54">
         <v>12</v>
@@ -4729,13 +4740,13 @@
       <c r="V15" s="74"/>
       <c r="W15" s="54"/>
       <c r="Y15" s="74" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Z15" s="54">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="74" t="s">
         <v>213</v>
       </c>
@@ -4787,7 +4798,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="74" t="s">
         <v>214</v>
       </c>
@@ -4823,7 +4834,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="74" t="s">
         <v>215</v>
       </c>
@@ -4833,7 +4844,7 @@
       <c r="D18" s="74"/>
       <c r="E18" s="54"/>
       <c r="G18" s="74" t="s">
-        <v>255</v>
+        <v>194</v>
       </c>
       <c r="H18" s="54">
         <v>15</v>
@@ -4849,19 +4860,19 @@
       <c r="S18" s="54"/>
       <c r="T18" s="54"/>
       <c r="V18" s="74" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="W18" s="54" t="s">
         <v>33</v>
       </c>
       <c r="Y18" s="74" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Z18">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="74" t="s">
         <v>186</v>
       </c>
@@ -4899,13 +4910,19 @@
         <v>5</v>
       </c>
       <c r="V19" s="75" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="W19" s="54" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Y19" s="74" t="s">
+        <v>258</v>
+      </c>
+      <c r="Z19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="74" t="s">
         <v>216</v>
       </c>
@@ -4948,8 +4965,14 @@
       <c r="W20" s="54" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Y20" t="s">
+        <v>277</v>
+      </c>
+      <c r="Z20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="74" t="s">
         <v>217</v>
       </c>
@@ -4998,14 +5021,14 @@
       <c r="W21" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="Y21" s="56" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z21" s="54">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Y21" t="s">
+        <v>230</v>
+      </c>
+      <c r="Z21">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="74" t="s">
         <v>188</v>
       </c>
@@ -5049,19 +5072,19 @@
         <v>34</v>
       </c>
       <c r="V22" s="74" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="W22" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="Y22" s="56" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z22" s="56" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Y22" s="74" t="s">
+        <v>276</v>
+      </c>
+      <c r="Z22">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="74"/>
       <c r="D23" s="75" t="s">
         <v>149</v>
@@ -5082,7 +5105,7 @@
         <v>35</v>
       </c>
       <c r="M23" s="75" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N23" s="54" t="s">
         <v>36</v>
@@ -5099,14 +5122,8 @@
       <c r="T23" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="Y23" s="74" t="s">
-        <v>238</v>
-      </c>
-      <c r="Z23" s="54" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D24" s="75" t="s">
         <v>123</v>
       </c>
@@ -5126,7 +5143,7 @@
         <v>36</v>
       </c>
       <c r="M24" s="74" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N24" s="54" t="s">
         <v>37</v>
@@ -5143,14 +5160,8 @@
       <c r="T24" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="Y24" s="75" t="s">
-        <v>269</v>
-      </c>
-      <c r="Z24" s="54" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="56" t="s">
         <v>78</v>
       </c>
@@ -5187,14 +5198,14 @@
       <c r="T25" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="Y25" s="75" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z25" s="54" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Y25" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z25" s="54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="56" t="s">
         <v>49</v>
       </c>
@@ -5207,14 +5218,14 @@
       <c r="H26" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="Y26" s="75" t="s">
-        <v>172</v>
-      </c>
-      <c r="Z26" s="54" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Y26" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z26" s="56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="74" t="s">
         <v>77</v>
       </c>
@@ -5222,63 +5233,79 @@
         <v>33</v>
       </c>
       <c r="G27" s="74" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H27" s="54" t="s">
         <v>37</v>
       </c>
       <c r="Y27" s="74" t="s">
-        <v>270</v>
+        <v>238</v>
       </c>
       <c r="Z27" s="54" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="75" t="s">
         <v>149</v>
       </c>
       <c r="B28" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="Y28" s="56"/>
-      <c r="Z28" s="56"/>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Y28" s="75" t="s">
+        <v>268</v>
+      </c>
+      <c r="Z28" s="54" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="75" t="s">
         <v>123</v>
       </c>
       <c r="B29" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="Y29" s="74"/>
-      <c r="Z29" s="54"/>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Y29" s="75" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z29" s="54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="75" t="s">
         <v>74</v>
       </c>
       <c r="B30" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="Y30" s="75"/>
-      <c r="Z30" s="54"/>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Y30" s="75" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z30" s="54" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="74" t="s">
         <v>245</v>
       </c>
       <c r="B31" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="Y31" s="75"/>
-      <c r="Z31" s="54"/>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Y31" s="74" t="s">
+        <v>269</v>
+      </c>
+      <c r="Z31" s="54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="Y32" s="75"/>
       <c r="Z32" s="54"/>
     </row>
-    <row r="33" spans="25:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="25:26" x14ac:dyDescent="0.25">
       <c r="Y33" s="74"/>
       <c r="Z33" s="54"/>
     </row>
@@ -5296,7 +5323,7 @@
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5310,7 +5337,7 @@
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5325,9 +5352,9 @@
       <selection activeCell="BP31" sqref="BP31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -5405,7 +5432,7 @@
       <c r="BO1" s="1"/>
       <c r="BP1" s="1"/>
     </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -5611,7 +5638,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>0</v>
       </c>
@@ -5693,7 +5720,7 @@
       <c r="BO3" s="16"/>
       <c r="BP3" s="16"/>
     </row>
-    <row r="4" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -5787,7 +5814,7 @@
       <c r="BO4" s="16"/>
       <c r="BP4" s="16"/>
     </row>
-    <row r="5" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -5893,7 +5920,7 @@
       </c>
       <c r="BP5" s="16"/>
     </row>
-    <row r="6" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -6025,7 +6052,7 @@
       </c>
       <c r="BP6" s="16"/>
     </row>
-    <row r="7" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>4</v>
       </c>
@@ -6179,7 +6206,7 @@
       </c>
       <c r="BP7" s="16"/>
     </row>
-    <row r="8" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -6361,7 +6388,7 @@
       </c>
       <c r="BP8" s="16"/>
     </row>
-    <row r="9" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -6557,7 +6584,7 @@
       </c>
       <c r="BP9" s="16"/>
     </row>
-    <row r="10" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>7</v>
       </c>
@@ -6763,7 +6790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>8</v>
       </c>
@@ -6969,7 +6996,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>9</v>
       </c>
@@ -7175,7 +7202,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>10</v>
       </c>
@@ -7381,7 +7408,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>11</v>
       </c>
@@ -7587,7 +7614,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>12</v>
       </c>
@@ -7793,7 +7820,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>13</v>
       </c>
@@ -7999,7 +8026,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>14</v>
       </c>
@@ -8205,7 +8232,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>15</v>
       </c>
@@ -8411,7 +8438,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>16</v>
       </c>
@@ -8617,7 +8644,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>17</v>
       </c>
@@ -8823,7 +8850,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>18</v>
       </c>
@@ -9029,7 +9056,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>19</v>
       </c>
@@ -9235,7 +9262,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>20</v>
       </c>
@@ -9441,7 +9468,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>21</v>
       </c>
@@ -9647,7 +9674,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>22</v>
       </c>
@@ -9853,7 +9880,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>23</v>
       </c>
@@ -10059,7 +10086,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>24</v>
       </c>
@@ -10265,7 +10292,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>25</v>
       </c>
@@ -10471,7 +10498,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>26</v>
       </c>
@@ -10677,7 +10704,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>27</v>
       </c>
@@ -10883,7 +10910,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>28</v>
       </c>
@@ -11102,9 +11129,9 @@
       <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>78</v>
       </c>
@@ -11112,7 +11139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
         <v>49</v>
       </c>
@@ -11120,7 +11147,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="74" t="s">
         <v>120</v>
       </c>
@@ -11128,7 +11155,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="75" t="s">
         <v>117</v>
       </c>
@@ -11136,7 +11163,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="75" t="s">
         <v>118</v>
       </c>
@@ -11144,7 +11171,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="75" t="s">
         <v>119</v>
       </c>
@@ -11152,7 +11179,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="74" t="s">
         <v>167</v>
       </c>
@@ -11160,16 +11187,16 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10" s="57"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D11" s="57"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12" s="57"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D13" s="57"/>
     </row>
   </sheetData>
@@ -11185,12 +11212,12 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.109375" style="54"/>
+    <col min="1" max="16384" width="9.140625" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>155</v>
       </c>
@@ -11198,7 +11225,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
         <v>78</v>
       </c>
@@ -11206,7 +11233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
         <v>137</v>
       </c>
@@ -11214,7 +11241,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
         <v>49</v>
       </c>
@@ -11222,7 +11249,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="74" t="s">
         <v>120</v>
       </c>
@@ -11231,7 +11258,7 @@
       </c>
       <c r="D5" s="57"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="75" t="s">
         <v>121</v>
       </c>
@@ -11240,7 +11267,7 @@
       </c>
       <c r="D6" s="57"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="75" t="s">
         <v>122</v>
       </c>
@@ -11249,7 +11276,7 @@
       </c>
       <c r="D7" s="57"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="75" t="s">
         <v>123</v>
       </c>
@@ -11258,7 +11285,7 @@
       </c>
       <c r="D8" s="57"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="74" t="s">
         <v>124</v>
       </c>
@@ -11266,7 +11293,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="56" t="s">
         <v>155</v>
       </c>
@@ -11274,7 +11301,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="56" t="s">
         <v>78</v>
       </c>
@@ -11282,7 +11309,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="56" t="s">
         <v>137</v>
       </c>
@@ -11290,7 +11317,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="56" t="s">
         <v>49</v>
       </c>
@@ -11299,7 +11326,7 @@
       </c>
       <c r="D14" s="57"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="74" t="s">
         <v>120</v>
       </c>
@@ -11308,7 +11335,7 @@
       </c>
       <c r="D15" s="57"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="75" t="s">
         <v>121</v>
       </c>
@@ -11317,7 +11344,7 @@
       </c>
       <c r="D16" s="57"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="75" t="s">
         <v>125</v>
       </c>
@@ -11326,7 +11353,7 @@
       </c>
       <c r="D17" s="57"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="75" t="s">
         <v>126</v>
       </c>
@@ -11335,7 +11362,7 @@
       </c>
       <c r="D18" s="57"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="74" t="s">
         <v>127</v>
       </c>
@@ -11344,7 +11371,7 @@
       </c>
       <c r="D19" s="57"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="56" t="s">
         <v>155</v>
       </c>
@@ -11352,7 +11379,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="56" t="s">
         <v>78</v>
       </c>
@@ -11360,7 +11387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="56" t="s">
         <v>137</v>
       </c>
@@ -11368,7 +11395,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="56" t="s">
         <v>49</v>
       </c>
@@ -11376,7 +11403,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="74" t="s">
         <v>120</v>
       </c>
@@ -11384,7 +11411,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="75" t="s">
         <v>121</v>
       </c>
@@ -11393,7 +11420,7 @@
       </c>
       <c r="D26" s="57"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="75" t="s">
         <v>122</v>
       </c>
@@ -11402,7 +11429,7 @@
       </c>
       <c r="D27" s="57"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="75" t="s">
         <v>128</v>
       </c>
@@ -11411,7 +11438,7 @@
       </c>
       <c r="D28" s="57"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="74" t="s">
         <v>129</v>
       </c>
@@ -11420,7 +11447,7 @@
       </c>
       <c r="D29" s="57"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="56" t="s">
         <v>155</v>
       </c>
@@ -11428,7 +11455,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="56" t="s">
         <v>78</v>
       </c>
@@ -11436,7 +11463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="56" t="s">
         <v>137</v>
       </c>
@@ -11444,7 +11471,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="56" t="s">
         <v>49</v>
       </c>
@@ -11452,7 +11479,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="74" t="s">
         <v>120</v>
       </c>
@@ -11460,7 +11487,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="75" t="s">
         <v>121</v>
       </c>
@@ -11469,7 +11496,7 @@
       </c>
       <c r="D36" s="57"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="75" t="s">
         <v>130</v>
       </c>
@@ -11478,7 +11505,7 @@
       </c>
       <c r="D37" s="57"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="75" t="s">
         <v>131</v>
       </c>
@@ -11487,7 +11514,7 @@
       </c>
       <c r="D38" s="57"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="74" t="s">
         <v>132</v>
       </c>
@@ -11496,7 +11523,7 @@
       </c>
       <c r="D39" s="57"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="56" t="s">
         <v>155</v>
       </c>
@@ -11504,7 +11531,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="56" t="s">
         <v>78</v>
       </c>
@@ -11512,7 +11539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="56" t="s">
         <v>137</v>
       </c>
@@ -11520,7 +11547,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="56" t="s">
         <v>49</v>
       </c>
@@ -11528,7 +11555,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="74" t="s">
         <v>133</v>
       </c>
@@ -11537,7 +11564,7 @@
       </c>
       <c r="D45" s="57"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="75" t="s">
         <v>134</v>
       </c>
@@ -11546,7 +11573,7 @@
       </c>
       <c r="D46" s="57"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="75" t="s">
         <v>73</v>
       </c>
@@ -11555,7 +11582,7 @@
       </c>
       <c r="D47" s="57"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="75" t="s">
         <v>135</v>
       </c>
@@ -11564,7 +11591,7 @@
       </c>
       <c r="D48" s="57"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="74" t="s">
         <v>136</v>
       </c>
@@ -11572,7 +11599,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="56" t="s">
         <v>155</v>
       </c>
@@ -11580,7 +11607,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="56" t="s">
         <v>78</v>
       </c>
@@ -11588,7 +11615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="56" t="s">
         <v>137</v>
       </c>
@@ -11596,7 +11623,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="56" t="s">
         <v>49</v>
       </c>
@@ -11604,7 +11631,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="74" t="s">
         <v>120</v>
       </c>
@@ -11612,7 +11639,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="75" t="s">
         <v>121</v>
       </c>
@@ -11621,7 +11648,7 @@
       </c>
       <c r="D56" s="57"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="75" t="s">
         <v>67</v>
       </c>
@@ -11630,7 +11657,7 @@
       </c>
       <c r="D57" s="57"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="75" t="s">
         <v>144</v>
       </c>
@@ -11639,7 +11666,7 @@
       </c>
       <c r="D58" s="57"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="74" t="s">
         <v>145</v>
       </c>
@@ -11648,7 +11675,7 @@
       </c>
       <c r="D59" s="57"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="56" t="s">
         <v>155</v>
       </c>
@@ -11656,7 +11683,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="56" t="s">
         <v>78</v>
       </c>
@@ -11664,7 +11691,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="56" t="s">
         <v>137</v>
       </c>
@@ -11672,7 +11699,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="56" t="s">
         <v>49</v>
       </c>
@@ -11680,7 +11707,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="74" t="s">
         <v>147</v>
       </c>
@@ -11688,7 +11715,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="75" t="s">
         <v>148</v>
       </c>
@@ -11696,7 +11723,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="75" t="s">
         <v>149</v>
       </c>
@@ -11705,7 +11732,7 @@
       </c>
       <c r="D67" s="57"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="75" t="s">
         <v>128</v>
       </c>
@@ -11714,7 +11741,7 @@
       </c>
       <c r="D68" s="57"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="74" t="s">
         <v>129</v>
       </c>
@@ -11723,10 +11750,10 @@
       </c>
       <c r="D69" s="57"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D70" s="57"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="56" t="s">
         <v>155</v>
       </c>
@@ -11735,7 +11762,7 @@
       </c>
       <c r="D71" s="57"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="56" t="s">
         <v>78</v>
       </c>
@@ -11743,7 +11770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="56" t="s">
         <v>137</v>
       </c>
@@ -11751,7 +11778,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="56" t="s">
         <v>49</v>
       </c>
@@ -11759,7 +11786,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="74" t="s">
         <v>120</v>
       </c>
@@ -11767,7 +11794,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="75" t="s">
         <v>121</v>
       </c>
@@ -11775,7 +11802,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="75" t="s">
         <v>67</v>
       </c>
@@ -11784,7 +11811,7 @@
       </c>
       <c r="D77" s="57"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="75" t="s">
         <v>165</v>
       </c>
@@ -11793,7 +11820,7 @@
       </c>
       <c r="D78" s="57"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="74" t="s">
         <v>166</v>
       </c>
@@ -11802,7 +11829,7 @@
       </c>
       <c r="D79" s="57"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="56" t="s">
         <v>155</v>
       </c>
@@ -11810,7 +11837,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="56" t="s">
         <v>78</v>
       </c>
@@ -11818,7 +11845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="56" t="s">
         <v>137</v>
       </c>
@@ -11826,7 +11853,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="56" t="s">
         <v>49</v>
       </c>
@@ -11834,7 +11861,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="74" t="s">
         <v>120</v>
       </c>
@@ -11842,7 +11869,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="75" t="s">
         <v>121</v>
       </c>
@@ -11851,7 +11878,7 @@
       </c>
       <c r="D86" s="57"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="75" t="s">
         <v>152</v>
       </c>
@@ -11860,7 +11887,7 @@
       </c>
       <c r="D87" s="57"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="75" t="s">
         <v>153</v>
       </c>
@@ -11869,7 +11896,7 @@
       </c>
       <c r="D88" s="57"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="74" t="s">
         <v>154</v>
       </c>
@@ -11892,9 +11919,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>78</v>
       </c>
@@ -11902,7 +11929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>49</v>
       </c>
@@ -11910,7 +11937,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>50</v>
       </c>
@@ -11918,7 +11945,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>51</v>
       </c>
@@ -11926,7 +11953,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
         <v>52</v>
       </c>
@@ -11934,7 +11961,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>53</v>
       </c>
@@ -11942,7 +11969,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>54</v>
       </c>
@@ -11965,18 +11992,18 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="60"/>
-    <col min="2" max="2" width="30.33203125" style="60" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.44140625" style="60" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.109375" style="60"/>
+    <col min="1" max="1" width="9.140625" style="60"/>
+    <col min="2" max="2" width="30.28515625" style="60" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.42578125" style="60" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="60"/>
     <col min="6" max="6" width="10" style="60" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" style="60" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="60"/>
+    <col min="7" max="7" width="10.85546875" style="60" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="60"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
         <v>93</v>
       </c>
@@ -11998,7 +12025,7 @@
       <c r="O1" s="61"/>
       <c r="P1" s="61"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="70">
         <v>1</v>
       </c>
@@ -12017,7 +12044,7 @@
       <c r="O2" s="77"/>
       <c r="P2" s="77"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="70">
         <v>2</v>
       </c>
@@ -12036,7 +12063,7 @@
       <c r="O3" s="77"/>
       <c r="P3" s="77"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="70">
         <v>3</v>
       </c>
@@ -12055,7 +12082,7 @@
       <c r="O4" s="77"/>
       <c r="P4" s="77"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="70">
         <v>4</v>
       </c>
@@ -12074,7 +12101,7 @@
       <c r="O5" s="77"/>
       <c r="P5" s="77"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="70">
         <v>5</v>
       </c>
@@ -12093,7 +12120,7 @@
       <c r="O6" s="77"/>
       <c r="P6" s="77"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="70">
         <v>6</v>
       </c>
@@ -12112,7 +12139,7 @@
       <c r="O7" s="77"/>
       <c r="P7" s="77"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="70">
         <v>7</v>
       </c>
@@ -12131,7 +12158,7 @@
       <c r="O8" s="77"/>
       <c r="P8" s="77"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="70">
         <v>8</v>
       </c>
@@ -12150,7 +12177,7 @@
       <c r="O9" s="77"/>
       <c r="P9" s="77"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="62"/>
       <c r="B10" s="62"/>
       <c r="C10" s="66"/>
@@ -12163,7 +12190,7 @@
       <c r="O10" s="77"/>
       <c r="P10" s="77"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="67" t="s">
         <v>92</v>
       </c>
@@ -12185,7 +12212,7 @@
       <c r="O11" s="77"/>
       <c r="P11" s="77"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="70">
         <v>1</v>
       </c>
@@ -12207,7 +12234,7 @@
       <c r="O12" s="77"/>
       <c r="P12" s="77"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="70">
         <v>2</v>
       </c>
@@ -12229,7 +12256,7 @@
       <c r="O13" s="77"/>
       <c r="P13" s="77"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="70">
         <v>3</v>
       </c>
@@ -12251,7 +12278,7 @@
       <c r="O14" s="59"/>
       <c r="P14" s="59"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="70">
         <v>4</v>
       </c>
@@ -12273,7 +12300,7 @@
       <c r="O15" s="59"/>
       <c r="P15" s="59"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="70">
         <v>5</v>
       </c>
@@ -12291,7 +12318,7 @@
       <c r="I16" s="63"/>
       <c r="J16" s="62"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" s="62"/>
       <c r="C17" s="66"/>
       <c r="D17" s="59"/>
@@ -12302,7 +12329,7 @@
       <c r="I17" s="63"/>
       <c r="J17" s="62"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="67" t="s">
         <v>99</v>
       </c>
@@ -12320,7 +12347,7 @@
       <c r="I18" s="63"/>
       <c r="J18" s="62"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="70">
         <v>1</v>
       </c>
@@ -12338,7 +12365,7 @@
       <c r="I19" s="63"/>
       <c r="J19" s="62"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="70">
         <v>2</v>
       </c>
@@ -12356,7 +12383,7 @@
       <c r="I20" s="63"/>
       <c r="J20" s="62"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="70">
         <v>3</v>
       </c>
@@ -12374,7 +12401,7 @@
       <c r="I21" s="63"/>
       <c r="J21" s="62"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="70">
         <v>4</v>
       </c>
@@ -12392,7 +12419,7 @@
       <c r="I22" s="63"/>
       <c r="J22" s="62"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="70">
         <v>5</v>
       </c>
@@ -12410,7 +12437,7 @@
       <c r="I23" s="63"/>
       <c r="J23" s="62"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="70">
         <v>6</v>
       </c>
@@ -12428,7 +12455,7 @@
       <c r="I24" s="63"/>
       <c r="J24" s="62"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="70">
         <v>7</v>
       </c>
@@ -12446,7 +12473,7 @@
       <c r="I25" s="63"/>
       <c r="J25" s="62"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="62"/>
       <c r="B26" s="62"/>
       <c r="C26" s="62"/>
@@ -12458,7 +12485,7 @@
       <c r="I26" s="63"/>
       <c r="J26" s="62"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="67" t="s">
         <v>107</v>
       </c>
@@ -12476,7 +12503,7 @@
       <c r="I27" s="63"/>
       <c r="J27" s="62"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="70">
         <v>1</v>
       </c>
@@ -12494,7 +12521,7 @@
       <c r="I28" s="63"/>
       <c r="J28" s="62"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="70">
         <v>2</v>
       </c>
@@ -12512,7 +12539,7 @@
       <c r="I29" s="64"/>
       <c r="J29" s="65"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="70">
         <v>3</v>
       </c>
@@ -12530,7 +12557,7 @@
       <c r="I30" s="59"/>
       <c r="J30" s="59"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="70">
         <v>4</v>
       </c>
@@ -12548,7 +12575,7 @@
       <c r="I31" s="59"/>
       <c r="J31" s="59"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="70">
         <v>5</v>
       </c>
@@ -12566,7 +12593,7 @@
       <c r="I32" s="59"/>
       <c r="J32" s="59"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="70">
         <v>6</v>
       </c>
@@ -12584,7 +12611,7 @@
       <c r="I33" s="59"/>
       <c r="J33" s="59"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="70">
         <v>7</v>
       </c>
@@ -12602,7 +12629,7 @@
       <c r="I34" s="59"/>
       <c r="J34" s="59"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="73">
         <v>8</v>
       </c>
@@ -12620,7 +12647,7 @@
       <c r="I35" s="59"/>
       <c r="J35" s="59"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D36" s="59"/>
       <c r="E36" s="59"/>
       <c r="F36" s="59"/>
@@ -12629,7 +12656,7 @@
       <c r="I36" s="59"/>
       <c r="J36" s="59"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="62"/>
       <c r="B37" s="62"/>
       <c r="C37" s="62"/>
@@ -12641,7 +12668,7 @@
       <c r="I37" s="59"/>
       <c r="J37" s="59"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="62"/>
       <c r="B38" s="62"/>
       <c r="C38" s="62"/>
@@ -12653,7 +12680,7 @@
       <c r="I38" s="59"/>
       <c r="J38" s="59"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="62"/>
       <c r="B39" s="62"/>
       <c r="C39" s="62"/>
@@ -12665,7 +12692,7 @@
       <c r="I39" s="59"/>
       <c r="J39" s="59"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="62"/>
       <c r="B40" s="62"/>
       <c r="C40" s="62"/>
@@ -12677,7 +12704,7 @@
       <c r="I40" s="59"/>
       <c r="J40" s="59"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="62"/>
       <c r="B41" s="62"/>
       <c r="C41" s="62"/>
@@ -12689,7 +12716,7 @@
       <c r="I41" s="59"/>
       <c r="J41" s="59"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="62"/>
       <c r="B42" s="62"/>
       <c r="C42" s="62"/>
@@ -12701,7 +12728,7 @@
       <c r="I42" s="59"/>
       <c r="J42" s="59"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="62"/>
       <c r="B43" s="62"/>
       <c r="C43" s="62"/>
@@ -12713,7 +12740,7 @@
       <c r="I43" s="59"/>
       <c r="J43" s="59"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="62"/>
       <c r="B44" s="62"/>
       <c r="C44" s="62"/>
@@ -12725,7 +12752,7 @@
       <c r="I44" s="59"/>
       <c r="J44" s="59"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="62"/>
       <c r="B45" s="62"/>
       <c r="C45" s="62"/>
@@ -12737,7 +12764,7 @@
       <c r="I45" s="59"/>
       <c r="J45" s="59"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="62"/>
       <c r="B46" s="62"/>
       <c r="C46" s="62"/>
@@ -12749,7 +12776,7 @@
       <c r="I46" s="59"/>
       <c r="J46" s="59"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="62"/>
       <c r="B47" s="62"/>
       <c r="C47" s="62"/>
@@ -12761,7 +12788,7 @@
       <c r="I47" s="59"/>
       <c r="J47" s="59"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="62"/>
       <c r="B48" s="62"/>
       <c r="C48" s="62"/>
@@ -12773,7 +12800,7 @@
       <c r="I48" s="59"/>
       <c r="J48" s="59"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="62"/>
       <c r="B49" s="62"/>
       <c r="C49" s="62"/>
@@ -12785,7 +12812,7 @@
       <c r="I49" s="59"/>
       <c r="J49" s="59"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="62"/>
       <c r="B50" s="62"/>
       <c r="C50" s="62"/>
@@ -12797,7 +12824,7 @@
       <c r="I50" s="59"/>
       <c r="J50" s="59"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="62"/>
       <c r="B51" s="62"/>
       <c r="C51" s="62"/>
@@ -12838,9 +12865,9 @@
       <selection activeCell="B7" sqref="A2:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>78</v>
       </c>
@@ -12848,7 +12875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>49</v>
       </c>
@@ -12856,7 +12883,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>80</v>
       </c>
@@ -12864,7 +12891,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>58</v>
       </c>
@@ -12872,7 +12899,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>57</v>
       </c>
@@ -12880,7 +12907,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>56</v>
       </c>
@@ -12888,7 +12915,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>54</v>
       </c>
@@ -12910,9 +12937,9 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>78</v>
       </c>
@@ -12920,7 +12947,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>49</v>
       </c>
@@ -12928,7 +12955,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>59</v>
       </c>
@@ -12936,7 +12963,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>60</v>
       </c>
@@ -12944,7 +12971,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>61</v>
       </c>
@@ -12952,7 +12979,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
         <v>62</v>
       </c>
@@ -12960,7 +12987,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>63</v>
       </c>
@@ -12982,9 +13009,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>78</v>
       </c>
@@ -12992,7 +13019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>49</v>
       </c>
@@ -13000,7 +13027,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>64</v>
       </c>
@@ -13008,7 +13035,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>65</v>
       </c>
@@ -13016,7 +13043,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
         <v>66</v>
       </c>
@@ -13024,7 +13051,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>67</v>
       </c>
@@ -13032,7 +13059,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="55" t="s">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
Finish Papi Kostik Calculation
</commit_message>
<xml_diff>
--- a/backend/src/data/test_norma.xlsx
+++ b/backend/src/data/test_norma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Important Files\Informatika ISTTS\_Semester 6\Kerja_Praktek\Project\adiputro_psytest_backend\backend\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4872067-B4E0-4C54-9DEE-4149461CD241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B14B2CB-90BD-4114-9C22-8DB6234D90C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="0" windowWidth="15375" windowHeight="7995" activeTab="15" xr2:uid="{28313136-274B-432F-8942-0592E5394583}"/>
+    <workbookView xWindow="4965" yWindow="690" windowWidth="15375" windowHeight="7995" firstSheet="12" activeTab="17" xr2:uid="{28313136-274B-432F-8942-0592E5394583}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="11" r:id="rId1"/>
@@ -30,7 +30,9 @@
     <sheet name="15" sheetId="9" r:id="rId15"/>
     <sheet name="16" sheetId="18" r:id="rId16"/>
     <sheet name="17" sheetId="16" r:id="rId17"/>
-    <sheet name="21" sheetId="17" r:id="rId18"/>
+    <sheet name="18" sheetId="19" r:id="rId18"/>
+    <sheet name="20" sheetId="20" r:id="rId19"/>
+    <sheet name="21" sheetId="17" r:id="rId20"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="409">
   <si>
     <t>College Student (Men)</t>
   </si>
@@ -884,6 +886,399 @@
   </si>
   <si>
     <t>0-4.9</t>
+  </si>
+  <si>
+    <t>Arah Kerja</t>
+  </si>
+  <si>
+    <t>Penyelesaian secara prestasi</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Peranan sebagai pekerja keras</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Hasrat untuk berprestasi</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Aspek</t>
+  </si>
+  <si>
+    <t>Faktor</t>
+  </si>
+  <si>
+    <t>Nomor</t>
+  </si>
+  <si>
+    <t>Benar(0) Ketika</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Analisis</t>
+  </si>
+  <si>
+    <t>Cenderung ragu-ragu dalam situasi pengambilan keputusan, cenderung ragu-ragu, menunda atau menghindari situasi pengambilan keputusan</t>
+  </si>
+  <si>
+    <t>Berhati-hati dan cenderung ragu-ragu</t>
+  </si>
+  <si>
+    <t>Cukup bertanggung jawab terhadap pekerjaan</t>
+  </si>
+  <si>
+    <t>Ketekunan, tanggung jawab terhadap tugas tinggi</t>
+  </si>
+  <si>
+    <t>Bekerja hanya untuk mengejar kesenangan saja bukan untuk memberikan suatu hasil yang baik</t>
+  </si>
+  <si>
+    <t>Kemauan bekerja keras tinggi</t>
+  </si>
+  <si>
+    <t>5-9</t>
+  </si>
+  <si>
+    <t>7-9</t>
+  </si>
+  <si>
+    <t>Fields</t>
+  </si>
+  <si>
+    <t>0-5</t>
+  </si>
+  <si>
+    <t>Mencerminkan ketidakpastian tujuan. Juga mencerminkan kepuasan dalam suatu pekerjaan, tidak perlu melanjutkan usaha untuk sukses</t>
+  </si>
+  <si>
+    <t>Tujuan-tujuan didefinisikan secara jelas, kebutuhan untuk sukses tinggi, ambisi pribadi tinggi</t>
+  </si>
+  <si>
+    <t>Kepemimpinan</t>
+  </si>
+  <si>
+    <t>Peran sebagai pimpinan</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Pengendalian orang lain</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Mudah dalam mengambil keputusan</t>
+  </si>
+  <si>
+    <t>Cenderung tidak suka aktif menggunakan orang lain dalam bekerja</t>
+  </si>
+  <si>
+    <t>Yaitu tingkat dimana seseorang memproyeksikan dirinya sebagai pemimpin suatu tingkat, dimana ia mencoba menggunakan orang lain untuk mencapai tujuannya. Nilai S menunjukkan apakah pola kepemimpinannya bersifat persuasive, demokratis, atau otoriter</t>
+  </si>
+  <si>
+    <t>Menurunnya keinginan untuk bertanggung jawab terhadap pekerjaan dan tindakan orang lain</t>
+  </si>
+  <si>
+    <t>Tingkat kebutuhan untuk menerima tanggung jawab orang lain, menjadi orang yang bertanggung jawab"</t>
+  </si>
+  <si>
+    <t>Ragu-ragu sampai penundaan/menolak situasi pengambilan keputusan</t>
+  </si>
+  <si>
+    <t>Berhati-hati sampai ragu-ragu dalam membuat keputusan</t>
+  </si>
+  <si>
+    <t>Mudah dan lancar sampai berhati-hati dalam membuat keputusan</t>
+  </si>
+  <si>
+    <t>Tidak ragu-ragu dalam proses pengambilan keputusan</t>
+  </si>
+  <si>
+    <t>Aktivitas</t>
+  </si>
+  <si>
+    <t>Melakukan segala sesuatu menurut kemauannya sendiri</t>
+  </si>
+  <si>
+    <t>4-9</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Tipe selalu sibuk</t>
+  </si>
+  <si>
+    <t>Tipe yang bersemangat</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Keaktifannya tergolong rendah, cenderung pasif (hanya duduk-duduk saja)</t>
+  </si>
+  <si>
+    <t>Keaktifannya secara fisik tergolong agak baik, cenderung tipe sportif</t>
+  </si>
+  <si>
+    <t>Pergaulan</t>
+  </si>
+  <si>
+    <t>Kebutuhan untuk mendapatkan perhatian</t>
+  </si>
+  <si>
+    <t>Pergaulan luas</t>
+  </si>
+  <si>
+    <t>Kebutuhan berkelompok</t>
+  </si>
+  <si>
+    <t>Kebutuhan untuk dekat dan menyayangi</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Cenderung pemalu, suka menyendiri</t>
+  </si>
+  <si>
+    <t>Rendah hati, tulus</t>
+  </si>
+  <si>
+    <t>Khusus, memiliki pola yang nyata</t>
+  </si>
+  <si>
+    <t>Membutuhkan perhatian yang nyata</t>
+  </si>
+  <si>
+    <t>Memiliki penilaian yang rendah terhadap hubungan sosial, cenderung kurang percaya pada orang lain</t>
+  </si>
+  <si>
+    <t>Tingkat kepercayaan dalam hubungan sosial tinggi, menyukai interaksi sosial</t>
+  </si>
+  <si>
+    <t>Selektif, secara umum melepaskan diri dari kelompok</t>
+  </si>
+  <si>
+    <t>Ada kebutuhan untuk diterima dan diakui tetapi tidak terlalu mudah dipengaruhi oleh kelompok</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Kebutuhan untuk disukai, diakui oleh semua orang. Mudah dipengaruhi kelompok</t>
+  </si>
+  <si>
+    <t>Tidak menyukai hubungan antar pribadi. Tidak menyukai interaksi perseorangan</t>
+  </si>
+  <si>
+    <t>Sadar akan kebutuhan antar pribadi tetapi dapat melepaskan diri dari orang lain/tidak terlalu tergantung</t>
+  </si>
+  <si>
+    <t>Ketergantungan yang sangat besar akan pengakuan dan penerimaan diri</t>
+  </si>
+  <si>
+    <t>Gaya Kerja</t>
+  </si>
+  <si>
+    <t>Tipe teoritikal</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Suka pekerjaan yang terperinci</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Tipe teratur</t>
+  </si>
+  <si>
+    <t>Kurang perhatian-praktis</t>
+  </si>
+  <si>
+    <t>Penekanan pada nialai-nilai penalaran tergolong tinggi</t>
+  </si>
+  <si>
+    <t>Menyadari kebutuhan akan kecermatan tetapi secara pribadi tidak berminat menangani hal-hal detail</t>
+  </si>
+  <si>
+    <t>Minat menangani hal-hal detail tergolong tinggi</t>
+  </si>
+  <si>
+    <t>Fleksibilitas sampai ketidak-teraturan</t>
+  </si>
+  <si>
+    <t>Tergolong teratur tetapi dengan fleksibilitas</t>
+  </si>
+  <si>
+    <t>Memiliki keteraturan yang sangat tinggi, cenderung kaku</t>
+  </si>
+  <si>
+    <t>Sifat</t>
+  </si>
+  <si>
+    <t>Hasrat untuk berubah</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>Pengendalian emosi</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Agresi</t>
+  </si>
+  <si>
+    <t>Tidak menyukai dan menolak perubahan. Cenderung menggunakan pendekatan-pendekatan tradisional</t>
+  </si>
+  <si>
+    <t>Tidak suka akan perubahan jika dipaksakan kepadanya</t>
+  </si>
+  <si>
+    <t>Mudah menyesuaikan diri</t>
+  </si>
+  <si>
+    <t>Pembuat perubahan yang selektif. Berpikir jauh ke depan</t>
+  </si>
+  <si>
+    <t>Mudah gelisah, mudah frustrasi mungkin karena segala sesuatu bergerak tidak cukup cepat</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Terbuka, cepat bereaksi, tidak memikirkan nilai dalam pengendalian diri</t>
+  </si>
+  <si>
+    <t>Terbuka</t>
+  </si>
+  <si>
+    <t>4-6</t>
+  </si>
+  <si>
+    <t>Memiliki pendekatan emosional yang seimbang. Mampu mengendalikan perasaannya</t>
+  </si>
+  <si>
+    <t>Sangat menepatkan nilai-nilai dalam setiap aktivitasnya. Kebutuhan pengendalian diri yang berlebih-lebihan, mungkin digunakan sebagai defence mechanisme</t>
+  </si>
+  <si>
+    <t>Selalu menghindari masalah. Cenderung mengabaikan situasi atau cenderung menolak untuk mengenali sesuatu sebagai sebuah masalah</t>
+  </si>
+  <si>
+    <t>Lebih menyukai lingkungan yang tenang. Menghindari konflik. Cenderung menunda masalah</t>
+  </si>
+  <si>
+    <t>Kukuh pendirian, cenderung keras kepala</t>
+  </si>
+  <si>
+    <t>Agresi pribadi yang berkaitan dengan pekerjaan, dorongan dan semangat bersaing</t>
+  </si>
+  <si>
+    <t>Agresif, cenderung defensive</t>
+  </si>
+  <si>
+    <t>Ketaatan</t>
+  </si>
+  <si>
+    <t>Dukungan terhadap atasan</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Kebutuhan taat pada aturan dan pengarahan</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Cenderung egois, kemungkinan bisa bersikap memberontak</t>
+  </si>
+  <si>
+    <t>Mengurus kepentingan diri sendiri</t>
+  </si>
+  <si>
+    <t>Setia terhadap perusahaan</t>
+  </si>
+  <si>
+    <t>Bersikap setia dan membantu secara pribadi, ada kemungkinan bantuannya bermotivasi politis</t>
+  </si>
+  <si>
+    <t>Berorientasi pada tujuan, mandiri</t>
+  </si>
+  <si>
+    <t>Kebutuhan akan pengarahan dan harapan yang dirumuskan untuknya</t>
+  </si>
+  <si>
+    <t>Meningkatnya orientasi terhadap tugas dan 'membutuhkan instruksi yang jelas</t>
+  </si>
+  <si>
+    <t>Total Atas</t>
+  </si>
+  <si>
+    <t>Total Bawah</t>
+  </si>
+  <si>
+    <t>Tergolong aktif secara internal dan mental</t>
   </si>
 </sst>
 </file>
@@ -936,7 +1331,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1012,6 +1407,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1117,7 +1518,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1292,10 +1693,32 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3622,7 +4045,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3908,7 +4331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80ECB89-F1E8-407D-8EEE-EA36F8B6F8A0}">
   <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
@@ -5303,7 +5726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E603AF88-1493-419E-A47E-525FA0DBED1A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -5314,11 +5737,2767 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7FC0B5A-8DF3-414E-B3BC-A3DB8B5A2D93}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70857D7D-8818-4C6D-9F42-45D186E1E399}">
+  <dimension ref="A2:BM35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>278</v>
+      </c>
+      <c r="G2" s="54" t="s">
+        <v>278</v>
+      </c>
+      <c r="K2" s="54" t="s">
+        <v>304</v>
+      </c>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54" t="s">
+        <v>304</v>
+      </c>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54" t="s">
+        <v>304</v>
+      </c>
+      <c r="R2" s="54"/>
+      <c r="U2" s="54" t="s">
+        <v>318</v>
+      </c>
+      <c r="V2" s="54"/>
+      <c r="W2" s="54"/>
+      <c r="X2" s="54" t="s">
+        <v>318</v>
+      </c>
+      <c r="Y2" s="54"/>
+      <c r="Z2" s="54"/>
+      <c r="AB2" s="54" t="s">
+        <v>339</v>
+      </c>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54" t="s">
+        <v>339</v>
+      </c>
+      <c r="AF2" s="54"/>
+      <c r="AH2" s="54" t="s">
+        <v>339</v>
+      </c>
+      <c r="AI2" s="54"/>
+      <c r="AJ2" s="54"/>
+      <c r="AK2" s="54" t="s">
+        <v>339</v>
+      </c>
+      <c r="AL2" s="54"/>
+      <c r="AO2" s="54" t="s">
+        <v>359</v>
+      </c>
+      <c r="AP2" s="54"/>
+      <c r="AQ2" s="54"/>
+      <c r="AR2" s="54" t="s">
+        <v>359</v>
+      </c>
+      <c r="AS2" s="54"/>
+      <c r="AU2" s="54" t="s">
+        <v>359</v>
+      </c>
+      <c r="AV2" s="54"/>
+      <c r="AY2" s="54" t="s">
+        <v>372</v>
+      </c>
+      <c r="AZ2" s="54"/>
+      <c r="BA2" s="54"/>
+      <c r="BB2" s="54" t="s">
+        <v>372</v>
+      </c>
+      <c r="BC2" s="54"/>
+      <c r="BD2" s="54"/>
+      <c r="BE2" s="54" t="s">
+        <v>372</v>
+      </c>
+      <c r="BF2" s="54"/>
+      <c r="BI2" s="54" t="s">
+        <v>394</v>
+      </c>
+      <c r="BJ2" s="54"/>
+      <c r="BK2" s="54"/>
+      <c r="BL2" s="54" t="s">
+        <v>394</v>
+      </c>
+      <c r="BM2" s="54"/>
+    </row>
+    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A3" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="B3" s="77" t="s">
+        <v>279</v>
+      </c>
+      <c r="D3" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="E3" s="77" t="s">
+        <v>281</v>
+      </c>
+      <c r="G3" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="H3" s="77" t="s">
+        <v>283</v>
+      </c>
+      <c r="K3" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="L3" s="83" t="s">
+        <v>305</v>
+      </c>
+      <c r="M3" s="54"/>
+      <c r="N3" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="O3" s="83" t="s">
+        <v>307</v>
+      </c>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="R3" s="83" t="s">
+        <v>309</v>
+      </c>
+      <c r="U3" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="V3" s="83" t="s">
+        <v>323</v>
+      </c>
+      <c r="W3" s="54"/>
+      <c r="X3" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="Y3" s="83" t="s">
+        <v>324</v>
+      </c>
+      <c r="Z3" s="54"/>
+      <c r="AB3" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="AC3" s="83" t="s">
+        <v>340</v>
+      </c>
+      <c r="AD3" s="54"/>
+      <c r="AE3" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="AF3" s="83" t="s">
+        <v>341</v>
+      </c>
+      <c r="AH3" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="AI3" s="83" t="s">
+        <v>342</v>
+      </c>
+      <c r="AJ3" s="54"/>
+      <c r="AK3" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="AL3" s="83" t="s">
+        <v>343</v>
+      </c>
+      <c r="AO3" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="AP3" s="83" t="s">
+        <v>360</v>
+      </c>
+      <c r="AQ3" s="54"/>
+      <c r="AR3" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="AS3" s="83" t="s">
+        <v>362</v>
+      </c>
+      <c r="AU3" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="AV3" s="83" t="s">
+        <v>364</v>
+      </c>
+      <c r="AY3" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="AZ3" s="83" t="s">
+        <v>373</v>
+      </c>
+      <c r="BA3" s="54"/>
+      <c r="BB3" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="BC3" s="83" t="s">
+        <v>375</v>
+      </c>
+      <c r="BD3" s="54"/>
+      <c r="BE3" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="BF3" s="83" t="s">
+        <v>377</v>
+      </c>
+      <c r="BI3" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="BJ3" s="83" t="s">
+        <v>395</v>
+      </c>
+      <c r="BK3" s="54"/>
+      <c r="BL3" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="BM3" s="83" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A4" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="D4" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="G4" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="K4" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="M4" s="54"/>
+      <c r="N4" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="U4" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="W4" s="54"/>
+      <c r="X4" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z4" s="54"/>
+      <c r="AB4" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="AC4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD4" s="54"/>
+      <c r="AE4" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="AF4" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="AH4" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="AI4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ4" s="54"/>
+      <c r="AK4" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="AL4" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="AO4" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="AP4" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="AQ4" s="54"/>
+      <c r="AR4" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="AS4" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="AU4" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="AV4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AY4" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="AZ4" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="BA4" s="54"/>
+      <c r="BB4" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="BC4" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="BD4" s="54"/>
+      <c r="BE4" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="BF4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="BI4" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="BJ4" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="BK4" s="54"/>
+      <c r="BL4" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="BM4" s="7" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A5" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="B5" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="D5" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="E5" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="G5" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="H5" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="K5" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="L5" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="M5" s="54"/>
+      <c r="N5" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="O5" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="R5" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="U5" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="V5" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="W5" s="54"/>
+      <c r="X5" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="Y5" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="Z5" s="54"/>
+      <c r="AB5" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="AC5" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="AD5" s="54"/>
+      <c r="AE5" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="AF5" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="AH5" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="AI5" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="AJ5" s="54"/>
+      <c r="AK5" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="AL5" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="AO5" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="AP5" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="AQ5" s="54"/>
+      <c r="AR5" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="AS5" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="AU5" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="AV5" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="AY5" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="AZ5" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="BA5" s="54"/>
+      <c r="BB5" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="BC5" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="BD5" s="54"/>
+      <c r="BE5" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="BF5" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="BI5" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="BJ5" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="BK5" s="54"/>
+      <c r="BL5" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="BM5" s="80" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A6" s="78">
+        <v>1</v>
+      </c>
+      <c r="B6" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="D6" s="78">
+        <v>1</v>
+      </c>
+      <c r="E6" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="G6" s="78">
+        <v>2</v>
+      </c>
+      <c r="H6" s="70" t="s">
+        <v>290</v>
+      </c>
+      <c r="K6" s="78">
+        <v>2</v>
+      </c>
+      <c r="L6" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="M6" s="54"/>
+      <c r="N6" s="78">
+        <v>13</v>
+      </c>
+      <c r="O6" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="78">
+        <v>23</v>
+      </c>
+      <c r="R6" s="70" t="s">
+        <v>290</v>
+      </c>
+      <c r="U6" s="86">
+        <v>34</v>
+      </c>
+      <c r="V6" s="86" t="s">
+        <v>290</v>
+      </c>
+      <c r="X6" s="86">
+        <v>45</v>
+      </c>
+      <c r="Y6" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AB6" s="78">
+        <v>24</v>
+      </c>
+      <c r="AC6" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AE6" s="78">
+        <v>56</v>
+      </c>
+      <c r="AF6" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AH6" s="78">
+        <v>35</v>
+      </c>
+      <c r="AI6" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AK6" s="78">
+        <v>46</v>
+      </c>
+      <c r="AL6" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AO6" s="78">
+        <v>67</v>
+      </c>
+      <c r="AP6" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AQ6" s="54"/>
+      <c r="AR6" s="78">
+        <v>78</v>
+      </c>
+      <c r="AS6" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AU6" s="78">
+        <v>89</v>
+      </c>
+      <c r="AV6" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AY6" s="78">
+        <v>57</v>
+      </c>
+      <c r="AZ6" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BA6" s="54"/>
+      <c r="BB6" s="78">
+        <v>89</v>
+      </c>
+      <c r="BC6" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="BD6" s="54"/>
+      <c r="BE6" s="78">
+        <v>68</v>
+      </c>
+      <c r="BF6" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BI6" s="78">
+        <v>79</v>
+      </c>
+      <c r="BJ6" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BK6" s="54"/>
+      <c r="BL6" s="78">
+        <v>90</v>
+      </c>
+      <c r="BM6" s="78" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A7" s="78">
+        <v>13</v>
+      </c>
+      <c r="B7" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="D7" s="78">
+        <v>11</v>
+      </c>
+      <c r="E7" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="G7" s="78">
+        <v>3</v>
+      </c>
+      <c r="H7" s="70" t="s">
+        <v>285</v>
+      </c>
+      <c r="K7" s="78">
+        <v>12</v>
+      </c>
+      <c r="L7" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="M7" s="54"/>
+      <c r="N7" s="78">
+        <v>3</v>
+      </c>
+      <c r="O7" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="78">
+        <v>33</v>
+      </c>
+      <c r="R7" s="70" t="s">
+        <v>290</v>
+      </c>
+      <c r="U7" s="86">
+        <v>44</v>
+      </c>
+      <c r="V7" s="86" t="s">
+        <v>290</v>
+      </c>
+      <c r="W7" s="74"/>
+      <c r="X7" s="87" t="s">
+        <v>329</v>
+      </c>
+      <c r="Y7" s="79" t="s">
+        <v>290</v>
+      </c>
+      <c r="Z7" s="74"/>
+      <c r="AA7" s="74"/>
+      <c r="AB7" s="78">
+        <v>14</v>
+      </c>
+      <c r="AC7" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AE7" s="78">
+        <v>66</v>
+      </c>
+      <c r="AF7" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AH7" s="78">
+        <v>25</v>
+      </c>
+      <c r="AI7" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AK7" s="78">
+        <v>36</v>
+      </c>
+      <c r="AL7" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AO7" s="78">
+        <v>77</v>
+      </c>
+      <c r="AP7" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AQ7" s="54"/>
+      <c r="AR7" s="78">
+        <v>88</v>
+      </c>
+      <c r="AS7" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AU7" s="78">
+        <v>88</v>
+      </c>
+      <c r="AV7" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AY7" s="78">
+        <v>47</v>
+      </c>
+      <c r="AZ7" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BA7" s="54"/>
+      <c r="BB7" s="78">
+        <v>78</v>
+      </c>
+      <c r="BC7" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="BD7" s="54"/>
+      <c r="BE7" s="78">
+        <v>58</v>
+      </c>
+      <c r="BF7" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BI7" s="78">
+        <v>69</v>
+      </c>
+      <c r="BJ7" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BK7" s="54"/>
+      <c r="BL7" s="78">
+        <v>80</v>
+      </c>
+      <c r="BM7" s="78" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A8" s="78">
+        <v>24</v>
+      </c>
+      <c r="B8" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="D8" s="78">
+        <v>21</v>
+      </c>
+      <c r="E8" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="G8" s="78">
+        <v>14</v>
+      </c>
+      <c r="H8" s="70" t="s">
+        <v>285</v>
+      </c>
+      <c r="K8" s="78">
+        <v>22</v>
+      </c>
+      <c r="L8" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="M8" s="54"/>
+      <c r="N8" s="78">
+        <v>4</v>
+      </c>
+      <c r="O8" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="78">
+        <v>43</v>
+      </c>
+      <c r="R8" s="70" t="s">
+        <v>290</v>
+      </c>
+      <c r="U8" s="87" t="s">
+        <v>325</v>
+      </c>
+      <c r="V8" s="87" t="s">
+        <v>290</v>
+      </c>
+      <c r="W8" s="74"/>
+      <c r="X8" s="87" t="s">
+        <v>330</v>
+      </c>
+      <c r="Y8" s="79" t="s">
+        <v>290</v>
+      </c>
+      <c r="Z8" s="74"/>
+      <c r="AA8" s="74"/>
+      <c r="AB8" s="78">
+        <v>4</v>
+      </c>
+      <c r="AC8" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AE8" s="78">
+        <v>76</v>
+      </c>
+      <c r="AF8" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AH8" s="78">
+        <v>15</v>
+      </c>
+      <c r="AI8" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AK8" s="78">
+        <v>26</v>
+      </c>
+      <c r="AL8" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AO8" s="78">
+        <v>87</v>
+      </c>
+      <c r="AP8" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AQ8" s="54"/>
+      <c r="AR8" s="78">
+        <v>87</v>
+      </c>
+      <c r="AS8" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AU8" s="78">
+        <v>77</v>
+      </c>
+      <c r="AV8" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AY8" s="78">
+        <v>37</v>
+      </c>
+      <c r="AZ8" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BA8" s="54"/>
+      <c r="BB8" s="78">
+        <v>67</v>
+      </c>
+      <c r="BC8" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="BD8" s="54"/>
+      <c r="BE8" s="78">
+        <v>48</v>
+      </c>
+      <c r="BF8" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BI8" s="78">
+        <v>59</v>
+      </c>
+      <c r="BJ8" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BK8" s="54"/>
+      <c r="BL8" s="78">
+        <v>70</v>
+      </c>
+      <c r="BM8" s="78" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A9" s="78">
+        <v>35</v>
+      </c>
+      <c r="B9" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="D9" s="78">
+        <v>31</v>
+      </c>
+      <c r="E9" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="G9" s="78">
+        <v>25</v>
+      </c>
+      <c r="H9" s="70" t="s">
+        <v>285</v>
+      </c>
+      <c r="K9" s="78">
+        <v>32</v>
+      </c>
+      <c r="L9" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="M9" s="54"/>
+      <c r="N9" s="78">
+        <v>15</v>
+      </c>
+      <c r="O9" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="78">
+        <v>53</v>
+      </c>
+      <c r="R9" s="70" t="s">
+        <v>290</v>
+      </c>
+      <c r="U9" s="86">
+        <v>64</v>
+      </c>
+      <c r="V9" s="86" t="s">
+        <v>290</v>
+      </c>
+      <c r="W9" s="74"/>
+      <c r="X9" s="87" t="s">
+        <v>331</v>
+      </c>
+      <c r="Y9" s="79" t="s">
+        <v>290</v>
+      </c>
+      <c r="Z9" s="74"/>
+      <c r="AA9" s="74"/>
+      <c r="AB9" s="78">
+        <v>5</v>
+      </c>
+      <c r="AC9" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AE9" s="78">
+        <v>86</v>
+      </c>
+      <c r="AF9" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AH9" s="78">
+        <v>5</v>
+      </c>
+      <c r="AI9" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AK9" s="78">
+        <v>16</v>
+      </c>
+      <c r="AL9" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AO9" s="78">
+        <v>86</v>
+      </c>
+      <c r="AP9" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AQ9" s="54"/>
+      <c r="AR9" s="78">
+        <v>76</v>
+      </c>
+      <c r="AS9" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AU9" s="78">
+        <v>66</v>
+      </c>
+      <c r="AV9" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AY9" s="78">
+        <v>27</v>
+      </c>
+      <c r="AZ9" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BA9" s="54"/>
+      <c r="BB9" s="78">
+        <v>56</v>
+      </c>
+      <c r="BC9" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="BD9" s="54"/>
+      <c r="BE9" s="78">
+        <v>38</v>
+      </c>
+      <c r="BF9" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BI9" s="78">
+        <v>49</v>
+      </c>
+      <c r="BJ9" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BK9" s="54"/>
+      <c r="BL9" s="78">
+        <v>60</v>
+      </c>
+      <c r="BM9" s="78" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A10" s="78">
+        <v>46</v>
+      </c>
+      <c r="B10" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="D10" s="78">
+        <v>41</v>
+      </c>
+      <c r="E10" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="G10" s="78">
+        <v>36</v>
+      </c>
+      <c r="H10" s="70" t="s">
+        <v>285</v>
+      </c>
+      <c r="K10" s="78">
+        <v>42</v>
+      </c>
+      <c r="L10" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="M10" s="54"/>
+      <c r="N10" s="78">
+        <v>26</v>
+      </c>
+      <c r="O10" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="78">
+        <v>63</v>
+      </c>
+      <c r="R10" s="70" t="s">
+        <v>290</v>
+      </c>
+      <c r="U10" s="86">
+        <v>74</v>
+      </c>
+      <c r="V10" s="86" t="s">
+        <v>290</v>
+      </c>
+      <c r="W10" s="74"/>
+      <c r="X10" s="87" t="s">
+        <v>332</v>
+      </c>
+      <c r="Y10" s="79" t="s">
+        <v>290</v>
+      </c>
+      <c r="Z10" s="74"/>
+      <c r="AA10" s="74"/>
+      <c r="AB10" s="78">
+        <v>16</v>
+      </c>
+      <c r="AC10" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AE10" s="78">
+        <v>85</v>
+      </c>
+      <c r="AF10" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AH10" s="78">
+        <v>6</v>
+      </c>
+      <c r="AI10" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AK10" s="78">
+        <v>6</v>
+      </c>
+      <c r="AL10" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="AO10" s="78">
+        <v>75</v>
+      </c>
+      <c r="AP10" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AQ10" s="54"/>
+      <c r="AR10" s="78">
+        <v>65</v>
+      </c>
+      <c r="AS10" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AU10" s="78">
+        <v>55</v>
+      </c>
+      <c r="AV10" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AY10" s="78">
+        <v>17</v>
+      </c>
+      <c r="AZ10" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BA10" s="54"/>
+      <c r="BB10" s="78">
+        <v>45</v>
+      </c>
+      <c r="BC10" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="BD10" s="54"/>
+      <c r="BE10" s="78">
+        <v>28</v>
+      </c>
+      <c r="BF10" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BI10" s="78">
+        <v>39</v>
+      </c>
+      <c r="BJ10" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BK10" s="54"/>
+      <c r="BL10" s="78">
+        <v>50</v>
+      </c>
+      <c r="BM10" s="78" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="11" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A11" s="78">
+        <v>57</v>
+      </c>
+      <c r="B11" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="D11" s="78">
+        <v>51</v>
+      </c>
+      <c r="E11" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="G11" s="78">
+        <v>47</v>
+      </c>
+      <c r="H11" s="70" t="s">
+        <v>285</v>
+      </c>
+      <c r="K11" s="78">
+        <v>52</v>
+      </c>
+      <c r="L11" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="M11" s="54"/>
+      <c r="N11" s="78">
+        <v>37</v>
+      </c>
+      <c r="O11" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="78">
+        <v>73</v>
+      </c>
+      <c r="R11" s="70" t="s">
+        <v>290</v>
+      </c>
+      <c r="U11" s="87" t="s">
+        <v>326</v>
+      </c>
+      <c r="V11" s="87" t="s">
+        <v>290</v>
+      </c>
+      <c r="W11" s="74"/>
+      <c r="X11" s="87" t="s">
+        <v>326</v>
+      </c>
+      <c r="Y11" s="79" t="s">
+        <v>285</v>
+      </c>
+      <c r="Z11" s="74"/>
+      <c r="AA11" s="74"/>
+      <c r="AB11" s="78">
+        <v>27</v>
+      </c>
+      <c r="AC11" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AE11" s="78">
+        <v>74</v>
+      </c>
+      <c r="AF11" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AH11" s="78">
+        <v>17</v>
+      </c>
+      <c r="AI11" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AK11" s="78">
+        <v>7</v>
+      </c>
+      <c r="AL11" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AO11" s="78">
+        <v>64</v>
+      </c>
+      <c r="AP11" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AQ11" s="54"/>
+      <c r="AR11" s="78">
+        <v>54</v>
+      </c>
+      <c r="AS11" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AU11" s="78">
+        <v>44</v>
+      </c>
+      <c r="AV11" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AY11" s="78">
+        <v>7</v>
+      </c>
+      <c r="AZ11" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BA11" s="54"/>
+      <c r="BB11" s="78">
+        <v>34</v>
+      </c>
+      <c r="BC11" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="BD11" s="54"/>
+      <c r="BE11" s="78">
+        <v>18</v>
+      </c>
+      <c r="BF11" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BI11" s="78">
+        <v>29</v>
+      </c>
+      <c r="BJ11" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BK11" s="54"/>
+      <c r="BL11" s="78">
+        <v>40</v>
+      </c>
+      <c r="BM11" s="78" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="12" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A12" s="78">
+        <v>68</v>
+      </c>
+      <c r="B12" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="D12" s="78">
+        <v>61</v>
+      </c>
+      <c r="E12" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="G12" s="78">
+        <v>58</v>
+      </c>
+      <c r="H12" s="70" t="s">
+        <v>285</v>
+      </c>
+      <c r="K12" s="78">
+        <v>62</v>
+      </c>
+      <c r="L12" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="M12" s="54"/>
+      <c r="N12" s="78">
+        <v>48</v>
+      </c>
+      <c r="O12" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="P12" s="54"/>
+      <c r="Q12" s="78">
+        <v>83</v>
+      </c>
+      <c r="R12" s="70" t="s">
+        <v>290</v>
+      </c>
+      <c r="U12" s="87" t="s">
+        <v>327</v>
+      </c>
+      <c r="V12" s="87" t="s">
+        <v>285</v>
+      </c>
+      <c r="W12" s="74"/>
+      <c r="X12" s="87" t="s">
+        <v>333</v>
+      </c>
+      <c r="Y12" s="79" t="s">
+        <v>285</v>
+      </c>
+      <c r="Z12" s="74"/>
+      <c r="AA12" s="74"/>
+      <c r="AB12" s="78">
+        <v>38</v>
+      </c>
+      <c r="AC12" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AE12" s="78">
+        <v>63</v>
+      </c>
+      <c r="AF12" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AH12" s="78">
+        <v>28</v>
+      </c>
+      <c r="AI12" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AK12" s="78">
+        <v>18</v>
+      </c>
+      <c r="AL12" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AO12" s="78">
+        <v>53</v>
+      </c>
+      <c r="AP12" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AQ12" s="54"/>
+      <c r="AR12" s="78">
+        <v>43</v>
+      </c>
+      <c r="AS12" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AU12" s="78">
+        <v>33</v>
+      </c>
+      <c r="AV12" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AY12" s="78">
+        <v>8</v>
+      </c>
+      <c r="AZ12" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="BA12" s="54"/>
+      <c r="BB12" s="78">
+        <v>23</v>
+      </c>
+      <c r="BC12" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="BD12" s="54"/>
+      <c r="BE12" s="78">
+        <v>8</v>
+      </c>
+      <c r="BF12" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BI12" s="78">
+        <v>19</v>
+      </c>
+      <c r="BJ12" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BK12" s="54"/>
+      <c r="BL12" s="78">
+        <v>30</v>
+      </c>
+      <c r="BM12" s="78" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="13" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A13" s="78">
+        <v>79</v>
+      </c>
+      <c r="B13" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="D13" s="78">
+        <v>71</v>
+      </c>
+      <c r="E13" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="G13" s="78">
+        <v>69</v>
+      </c>
+      <c r="H13" s="70" t="s">
+        <v>285</v>
+      </c>
+      <c r="K13" s="78">
+        <v>72</v>
+      </c>
+      <c r="L13" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="M13" s="54"/>
+      <c r="N13" s="78">
+        <v>59</v>
+      </c>
+      <c r="O13" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="P13" s="54"/>
+      <c r="Q13" s="78">
+        <v>82</v>
+      </c>
+      <c r="R13" s="70" t="s">
+        <v>285</v>
+      </c>
+      <c r="U13" s="87" t="s">
+        <v>328</v>
+      </c>
+      <c r="V13" s="87" t="s">
+        <v>285</v>
+      </c>
+      <c r="W13" s="74"/>
+      <c r="X13" s="87" t="s">
+        <v>334</v>
+      </c>
+      <c r="Y13" s="79" t="s">
+        <v>285</v>
+      </c>
+      <c r="Z13" s="74"/>
+      <c r="AA13" s="74"/>
+      <c r="AB13" s="78">
+        <v>49</v>
+      </c>
+      <c r="AC13" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AE13" s="78">
+        <v>52</v>
+      </c>
+      <c r="AF13" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AH13" s="78">
+        <v>39</v>
+      </c>
+      <c r="AI13" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AK13" s="78">
+        <v>29</v>
+      </c>
+      <c r="AL13" s="70" t="s">
+        <v>285</v>
+      </c>
+      <c r="AO13" s="78">
+        <v>42</v>
+      </c>
+      <c r="AP13" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AQ13" s="54"/>
+      <c r="AR13" s="78">
+        <v>32</v>
+      </c>
+      <c r="AS13" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AU13" s="78">
+        <v>22</v>
+      </c>
+      <c r="AV13" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AY13" s="78">
+        <v>19</v>
+      </c>
+      <c r="AZ13" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="BA13" s="54"/>
+      <c r="BB13" s="78">
+        <v>12</v>
+      </c>
+      <c r="BC13" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="BD13" s="54"/>
+      <c r="BE13" s="78">
+        <v>9</v>
+      </c>
+      <c r="BF13" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="BI13" s="78">
+        <v>9</v>
+      </c>
+      <c r="BJ13" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="BK13" s="54"/>
+      <c r="BL13" s="78">
+        <v>20</v>
+      </c>
+      <c r="BM13" s="78" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="14" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A14" s="78">
+        <v>90</v>
+      </c>
+      <c r="B14" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="D14" s="78">
+        <v>81</v>
+      </c>
+      <c r="E14" s="78" t="s">
+        <v>290</v>
+      </c>
+      <c r="G14" s="78">
+        <v>80</v>
+      </c>
+      <c r="H14" s="70" t="s">
+        <v>285</v>
+      </c>
+      <c r="K14" s="78">
+        <v>81</v>
+      </c>
+      <c r="L14" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="M14" s="54"/>
+      <c r="N14" s="78">
+        <v>70</v>
+      </c>
+      <c r="O14" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="78">
+        <v>71</v>
+      </c>
+      <c r="R14" s="70" t="s">
+        <v>285</v>
+      </c>
+      <c r="U14" s="86">
+        <v>61</v>
+      </c>
+      <c r="V14" s="87" t="s">
+        <v>285</v>
+      </c>
+      <c r="W14" s="74"/>
+      <c r="X14" s="87" t="s">
+        <v>335</v>
+      </c>
+      <c r="Y14" s="79" t="s">
+        <v>285</v>
+      </c>
+      <c r="Z14" s="74"/>
+      <c r="AA14" s="74"/>
+      <c r="AB14" s="78">
+        <v>60</v>
+      </c>
+      <c r="AC14" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AE14" s="78">
+        <v>41</v>
+      </c>
+      <c r="AF14" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AH14" s="78">
+        <v>50</v>
+      </c>
+      <c r="AI14" s="70" t="s">
+        <v>285</v>
+      </c>
+      <c r="AK14" s="78">
+        <v>40</v>
+      </c>
+      <c r="AL14" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AO14" s="78">
+        <v>31</v>
+      </c>
+      <c r="AP14" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AQ14" s="54"/>
+      <c r="AR14" s="78">
+        <v>21</v>
+      </c>
+      <c r="AS14" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AU14" s="78">
+        <v>11</v>
+      </c>
+      <c r="AV14" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="AY14" s="78">
+        <v>30</v>
+      </c>
+      <c r="AZ14" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="BA14" s="54"/>
+      <c r="BB14" s="78">
+        <v>1</v>
+      </c>
+      <c r="BC14" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="BD14" s="54"/>
+      <c r="BE14" s="78">
+        <v>20</v>
+      </c>
+      <c r="BF14" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="BI14" s="78">
+        <v>10</v>
+      </c>
+      <c r="BJ14" s="78" t="s">
+        <v>285</v>
+      </c>
+      <c r="BK14" s="54"/>
+      <c r="BL14" s="78">
+        <v>10</v>
+      </c>
+      <c r="BM14" s="78" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="15" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="54"/>
+      <c r="O15" s="54"/>
+      <c r="P15" s="54"/>
+      <c r="Q15" s="54"/>
+      <c r="R15" s="54"/>
+      <c r="W15" s="74"/>
+      <c r="X15" s="74"/>
+      <c r="Y15" s="74"/>
+      <c r="Z15" s="74"/>
+      <c r="AA15" s="74"/>
+      <c r="AO15" s="54"/>
+      <c r="AP15" s="54"/>
+      <c r="AQ15" s="54"/>
+      <c r="AR15" s="54"/>
+      <c r="AS15" s="54"/>
+      <c r="AU15" s="54"/>
+      <c r="AV15" s="54"/>
+      <c r="AY15" s="54"/>
+      <c r="AZ15" s="54"/>
+      <c r="BA15" s="54"/>
+      <c r="BB15" s="54"/>
+      <c r="BC15" s="54"/>
+      <c r="BD15" s="54"/>
+      <c r="BE15" s="54"/>
+      <c r="BF15" s="54"/>
+      <c r="BI15" s="54"/>
+      <c r="BJ15" s="54"/>
+      <c r="BK15" s="54"/>
+      <c r="BL15" s="54"/>
+      <c r="BM15" s="54"/>
+    </row>
+    <row r="16" spans="1:65" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="80" t="s">
+        <v>300</v>
+      </c>
+      <c r="B16" s="78">
+        <v>4</v>
+      </c>
+      <c r="D16" s="80" t="s">
+        <v>300</v>
+      </c>
+      <c r="E16" s="78">
+        <v>2</v>
+      </c>
+      <c r="G16" s="80" t="s">
+        <v>300</v>
+      </c>
+      <c r="H16" s="78">
+        <v>2</v>
+      </c>
+      <c r="K16" s="84" t="s">
+        <v>300</v>
+      </c>
+      <c r="L16" s="79" t="s">
+        <v>336</v>
+      </c>
+      <c r="M16" s="74"/>
+      <c r="N16" s="84" t="s">
+        <v>300</v>
+      </c>
+      <c r="O16" s="79">
+        <v>2</v>
+      </c>
+      <c r="P16" s="74"/>
+      <c r="Q16" s="84" t="s">
+        <v>300</v>
+      </c>
+      <c r="R16" s="79" t="s">
+        <v>321</v>
+      </c>
+      <c r="S16" s="74"/>
+      <c r="T16" s="74"/>
+      <c r="U16" s="84" t="s">
+        <v>300</v>
+      </c>
+      <c r="V16" s="79" t="s">
+        <v>336</v>
+      </c>
+      <c r="W16" s="74"/>
+      <c r="X16" s="84" t="s">
+        <v>300</v>
+      </c>
+      <c r="Y16" s="79" t="s">
+        <v>336</v>
+      </c>
+      <c r="Z16" s="74"/>
+      <c r="AA16" s="74"/>
+      <c r="AB16" s="84" t="s">
+        <v>300</v>
+      </c>
+      <c r="AC16" s="79" t="s">
+        <v>321</v>
+      </c>
+      <c r="AD16" s="74"/>
+      <c r="AE16" s="84" t="s">
+        <v>300</v>
+      </c>
+      <c r="AF16" s="79" t="s">
+        <v>336</v>
+      </c>
+      <c r="AG16" s="74"/>
+      <c r="AH16" s="84" t="s">
+        <v>300</v>
+      </c>
+      <c r="AI16" s="79" t="s">
+        <v>354</v>
+      </c>
+      <c r="AJ16" s="74"/>
+      <c r="AK16" s="84" t="s">
+        <v>300</v>
+      </c>
+      <c r="AL16" s="79" t="s">
+        <v>354</v>
+      </c>
+      <c r="AM16" s="74"/>
+      <c r="AN16" s="74"/>
+      <c r="AO16" s="84" t="s">
+        <v>300</v>
+      </c>
+      <c r="AP16" s="79" t="s">
+        <v>336</v>
+      </c>
+      <c r="AQ16" s="74"/>
+      <c r="AR16" s="84" t="s">
+        <v>300</v>
+      </c>
+      <c r="AS16" s="79" t="s">
+        <v>336</v>
+      </c>
+      <c r="AU16" s="84" t="s">
+        <v>300</v>
+      </c>
+      <c r="AV16" s="79" t="s">
+        <v>354</v>
+      </c>
+      <c r="AY16" s="84" t="s">
+        <v>300</v>
+      </c>
+      <c r="AZ16" s="79" t="s">
+        <v>383</v>
+      </c>
+      <c r="BA16" s="74"/>
+      <c r="BB16" s="84" t="s">
+        <v>300</v>
+      </c>
+      <c r="BC16" s="79" t="s">
+        <v>321</v>
+      </c>
+      <c r="BE16" s="84" t="s">
+        <v>300</v>
+      </c>
+      <c r="BF16" s="79" t="s">
+        <v>383</v>
+      </c>
+      <c r="BI16" s="84" t="s">
+        <v>300</v>
+      </c>
+      <c r="BJ16" s="79" t="s">
+        <v>321</v>
+      </c>
+      <c r="BK16" s="74"/>
+      <c r="BL16" s="84" t="s">
+        <v>300</v>
+      </c>
+      <c r="BM16" s="79" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="17" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A17" s="80" t="s">
+        <v>291</v>
+      </c>
+      <c r="B17" s="80" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="80" t="s">
+        <v>291</v>
+      </c>
+      <c r="E17" s="80" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" s="80" t="s">
+        <v>291</v>
+      </c>
+      <c r="H17" s="80" t="s">
+        <v>82</v>
+      </c>
+      <c r="K17" s="84" t="s">
+        <v>291</v>
+      </c>
+      <c r="L17" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="M17" s="74"/>
+      <c r="N17" s="84" t="s">
+        <v>291</v>
+      </c>
+      <c r="O17" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="P17" s="74"/>
+      <c r="Q17" s="84" t="s">
+        <v>291</v>
+      </c>
+      <c r="R17" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="S17" s="74"/>
+      <c r="T17" s="74"/>
+      <c r="U17" s="84" t="s">
+        <v>291</v>
+      </c>
+      <c r="V17" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="W17" s="74"/>
+      <c r="X17" s="84" t="s">
+        <v>291</v>
+      </c>
+      <c r="Y17" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z17" s="74"/>
+      <c r="AA17" s="74"/>
+      <c r="AB17" s="84" t="s">
+        <v>291</v>
+      </c>
+      <c r="AC17" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD17" s="74"/>
+      <c r="AE17" s="84" t="s">
+        <v>291</v>
+      </c>
+      <c r="AF17" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG17" s="74"/>
+      <c r="AH17" s="84" t="s">
+        <v>291</v>
+      </c>
+      <c r="AI17" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ17" s="74"/>
+      <c r="AK17" s="84" t="s">
+        <v>291</v>
+      </c>
+      <c r="AL17" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM17" s="74"/>
+      <c r="AN17" s="74"/>
+      <c r="AO17" s="84" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP17" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ17" s="74"/>
+      <c r="AR17" s="84" t="s">
+        <v>291</v>
+      </c>
+      <c r="AS17" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="AU17" s="84" t="s">
+        <v>291</v>
+      </c>
+      <c r="AV17" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="AY17" s="84" t="s">
+        <v>291</v>
+      </c>
+      <c r="AZ17" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="BA17" s="74"/>
+      <c r="BB17" s="84" t="s">
+        <v>291</v>
+      </c>
+      <c r="BC17" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="BD17" s="54"/>
+      <c r="BE17" s="84" t="s">
+        <v>291</v>
+      </c>
+      <c r="BF17" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="BI17" s="84" t="s">
+        <v>291</v>
+      </c>
+      <c r="BJ17" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="BK17" s="74"/>
+      <c r="BL17" s="84" t="s">
+        <v>291</v>
+      </c>
+      <c r="BM17" s="84" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A18" s="79" t="s">
+        <v>239</v>
+      </c>
+      <c r="B18" s="78" t="s">
+        <v>292</v>
+      </c>
+      <c r="D18" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="78" t="s">
+        <v>296</v>
+      </c>
+      <c r="G18" s="79" t="s">
+        <v>301</v>
+      </c>
+      <c r="H18" s="78" t="s">
+        <v>302</v>
+      </c>
+      <c r="K18" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="L18" s="79" t="s">
+        <v>310</v>
+      </c>
+      <c r="M18" s="74"/>
+      <c r="N18" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="O18" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="P18" s="74"/>
+      <c r="Q18" s="79" t="s">
+        <v>239</v>
+      </c>
+      <c r="R18" s="79" t="s">
+        <v>314</v>
+      </c>
+      <c r="S18" s="74"/>
+      <c r="T18" s="74"/>
+      <c r="U18" s="85" t="s">
+        <v>239</v>
+      </c>
+      <c r="V18" s="78" t="s">
+        <v>319</v>
+      </c>
+      <c r="W18" s="74"/>
+      <c r="X18" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y18" s="79" t="s">
+        <v>337</v>
+      </c>
+      <c r="Z18" s="74"/>
+      <c r="AA18" s="74"/>
+      <c r="AB18" s="79" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC18" s="79" t="s">
+        <v>346</v>
+      </c>
+      <c r="AD18" s="74"/>
+      <c r="AE18" s="79" t="s">
+        <v>301</v>
+      </c>
+      <c r="AF18" s="79" t="s">
+        <v>350</v>
+      </c>
+      <c r="AG18" s="74"/>
+      <c r="AH18" s="79" t="s">
+        <v>239</v>
+      </c>
+      <c r="AI18" s="79" t="s">
+        <v>352</v>
+      </c>
+      <c r="AJ18" s="74"/>
+      <c r="AK18" s="79" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL18" s="79" t="s">
+        <v>356</v>
+      </c>
+      <c r="AM18" s="74"/>
+      <c r="AN18" s="74"/>
+      <c r="AO18" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP18" s="79" t="s">
+        <v>365</v>
+      </c>
+      <c r="AQ18" s="74"/>
+      <c r="AR18" s="79" t="s">
+        <v>239</v>
+      </c>
+      <c r="AS18" s="79" t="s">
+        <v>367</v>
+      </c>
+      <c r="AU18" s="89" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV18" s="78" t="s">
+        <v>369</v>
+      </c>
+      <c r="AY18" s="79" t="s">
+        <v>120</v>
+      </c>
+      <c r="AZ18" s="79" t="s">
+        <v>378</v>
+      </c>
+      <c r="BA18" s="74"/>
+      <c r="BB18" s="79" t="s">
+        <v>147</v>
+      </c>
+      <c r="BC18" s="79" t="s">
+        <v>384</v>
+      </c>
+      <c r="BD18" s="74"/>
+      <c r="BE18" s="79" t="s">
+        <v>120</v>
+      </c>
+      <c r="BF18" s="79" t="s">
+        <v>389</v>
+      </c>
+      <c r="BI18" s="79" t="s">
+        <v>147</v>
+      </c>
+      <c r="BJ18" s="79" t="s">
+        <v>399</v>
+      </c>
+      <c r="BK18" s="74"/>
+      <c r="BL18" s="79" t="s">
+        <v>239</v>
+      </c>
+      <c r="BM18" s="79" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="19" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A19" s="79" t="s">
+        <v>242</v>
+      </c>
+      <c r="B19" s="78" t="s">
+        <v>293</v>
+      </c>
+      <c r="D19" s="79" t="s">
+        <v>298</v>
+      </c>
+      <c r="E19" s="78" t="s">
+        <v>297</v>
+      </c>
+      <c r="G19" s="79" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="78" t="s">
+        <v>303</v>
+      </c>
+      <c r="K19" s="79" t="s">
+        <v>298</v>
+      </c>
+      <c r="L19" s="79" t="s">
+        <v>311</v>
+      </c>
+      <c r="M19" s="74"/>
+      <c r="N19" s="79" t="s">
+        <v>298</v>
+      </c>
+      <c r="O19" s="79" t="s">
+        <v>313</v>
+      </c>
+      <c r="P19" s="74"/>
+      <c r="Q19" s="79" t="s">
+        <v>242</v>
+      </c>
+      <c r="R19" s="79" t="s">
+        <v>315</v>
+      </c>
+      <c r="S19" s="74"/>
+      <c r="T19" s="74"/>
+      <c r="U19" s="79" t="s">
+        <v>320</v>
+      </c>
+      <c r="V19" s="79" t="s">
+        <v>408</v>
+      </c>
+      <c r="W19" s="74"/>
+      <c r="X19" s="79" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y19" s="79" t="s">
+        <v>338</v>
+      </c>
+      <c r="Z19" s="74"/>
+      <c r="AA19" s="74"/>
+      <c r="AB19" s="79" t="s">
+        <v>264</v>
+      </c>
+      <c r="AC19" s="79" t="s">
+        <v>347</v>
+      </c>
+      <c r="AD19" s="74"/>
+      <c r="AE19" s="79" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF19" s="79" t="s">
+        <v>351</v>
+      </c>
+      <c r="AG19" s="74"/>
+      <c r="AH19" s="79" t="s">
+        <v>265</v>
+      </c>
+      <c r="AI19" s="79" t="s">
+        <v>353</v>
+      </c>
+      <c r="AJ19" s="74"/>
+      <c r="AK19" s="79" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL19" s="79" t="s">
+        <v>357</v>
+      </c>
+      <c r="AM19" s="74"/>
+      <c r="AN19" s="74"/>
+      <c r="AO19" s="79" t="s">
+        <v>298</v>
+      </c>
+      <c r="AP19" s="79" t="s">
+        <v>366</v>
+      </c>
+      <c r="AQ19" s="74"/>
+      <c r="AR19" s="79" t="s">
+        <v>320</v>
+      </c>
+      <c r="AS19" s="79" t="s">
+        <v>368</v>
+      </c>
+      <c r="AU19" s="79" t="s">
+        <v>121</v>
+      </c>
+      <c r="AV19" s="78" t="s">
+        <v>370</v>
+      </c>
+      <c r="AY19" s="79" t="s">
+        <v>117</v>
+      </c>
+      <c r="AZ19" s="79" t="s">
+        <v>379</v>
+      </c>
+      <c r="BA19" s="74"/>
+      <c r="BB19" s="79" t="s">
+        <v>264</v>
+      </c>
+      <c r="BC19" s="79" t="s">
+        <v>385</v>
+      </c>
+      <c r="BD19" s="74"/>
+      <c r="BE19" s="79" t="s">
+        <v>117</v>
+      </c>
+      <c r="BF19" s="79" t="s">
+        <v>390</v>
+      </c>
+      <c r="BI19" s="79" t="s">
+        <v>264</v>
+      </c>
+      <c r="BJ19" s="79" t="s">
+        <v>400</v>
+      </c>
+      <c r="BK19" s="74"/>
+      <c r="BL19" s="79" t="s">
+        <v>265</v>
+      </c>
+      <c r="BM19" s="79" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="20" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A20" s="79" t="s">
+        <v>243</v>
+      </c>
+      <c r="B20" s="78" t="s">
+        <v>294</v>
+      </c>
+      <c r="D20" s="81"/>
+      <c r="E20" s="82"/>
+      <c r="K20" s="74"/>
+      <c r="L20" s="74"/>
+      <c r="M20" s="74"/>
+      <c r="N20" s="74"/>
+      <c r="O20" s="74"/>
+      <c r="P20" s="74"/>
+      <c r="Q20" s="79" t="s">
+        <v>76</v>
+      </c>
+      <c r="R20" s="79" t="s">
+        <v>316</v>
+      </c>
+      <c r="S20" s="74"/>
+      <c r="T20" s="74"/>
+      <c r="U20" s="74"/>
+      <c r="V20" s="74"/>
+      <c r="W20" s="74"/>
+      <c r="X20" s="74"/>
+      <c r="Y20" s="74"/>
+      <c r="Z20" s="74"/>
+      <c r="AA20" s="74"/>
+      <c r="AB20" s="79" t="s">
+        <v>265</v>
+      </c>
+      <c r="AC20" s="79" t="s">
+        <v>348</v>
+      </c>
+      <c r="AD20" s="74"/>
+      <c r="AE20" s="74"/>
+      <c r="AF20" s="74"/>
+      <c r="AG20" s="74"/>
+      <c r="AH20" s="79" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI20" s="79" t="s">
+        <v>355</v>
+      </c>
+      <c r="AJ20" s="74"/>
+      <c r="AK20" s="79" t="s">
+        <v>298</v>
+      </c>
+      <c r="AL20" s="79" t="s">
+        <v>358</v>
+      </c>
+      <c r="AM20" s="74"/>
+      <c r="AN20" s="74"/>
+      <c r="AO20" s="74"/>
+      <c r="AP20" s="74"/>
+      <c r="AQ20" s="74"/>
+      <c r="AR20" s="74"/>
+      <c r="AS20" s="74"/>
+      <c r="AU20" s="79" t="s">
+        <v>67</v>
+      </c>
+      <c r="AV20" s="78" t="s">
+        <v>371</v>
+      </c>
+      <c r="AY20" s="79" t="s">
+        <v>243</v>
+      </c>
+      <c r="AZ20" s="79" t="s">
+        <v>380</v>
+      </c>
+      <c r="BA20" s="74"/>
+      <c r="BB20" s="79" t="s">
+        <v>386</v>
+      </c>
+      <c r="BC20" s="79" t="s">
+        <v>387</v>
+      </c>
+      <c r="BD20" s="74"/>
+      <c r="BE20" s="79" t="s">
+        <v>205</v>
+      </c>
+      <c r="BF20" s="79" t="s">
+        <v>391</v>
+      </c>
+      <c r="BI20" s="79" t="s">
+        <v>265</v>
+      </c>
+      <c r="BJ20" s="79" t="s">
+        <v>401</v>
+      </c>
+      <c r="BK20" s="74"/>
+      <c r="BL20" s="79" t="s">
+        <v>67</v>
+      </c>
+      <c r="BM20" s="79" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="21" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A21" s="79" t="s">
+        <v>299</v>
+      </c>
+      <c r="B21" s="78" t="s">
+        <v>295</v>
+      </c>
+      <c r="D21" s="81"/>
+      <c r="E21" s="82"/>
+      <c r="K21" s="74"/>
+      <c r="L21" s="74"/>
+      <c r="M21" s="74"/>
+      <c r="N21" s="74"/>
+      <c r="O21" s="74"/>
+      <c r="P21" s="74"/>
+      <c r="Q21" s="79" t="s">
+        <v>126</v>
+      </c>
+      <c r="R21" s="79" t="s">
+        <v>317</v>
+      </c>
+      <c r="S21" s="74"/>
+      <c r="T21" s="74"/>
+      <c r="W21" s="74"/>
+      <c r="X21" s="74"/>
+      <c r="Y21" s="74"/>
+      <c r="Z21" s="74"/>
+      <c r="AA21" s="74"/>
+      <c r="AB21" s="79" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC21" s="79" t="s">
+        <v>349</v>
+      </c>
+      <c r="AD21" s="74"/>
+      <c r="AE21" s="74"/>
+      <c r="AF21" s="74"/>
+      <c r="AG21" s="74"/>
+      <c r="AH21" s="74"/>
+      <c r="AI21" s="74"/>
+      <c r="AJ21" s="74"/>
+      <c r="AK21" s="74"/>
+      <c r="AL21" s="74"/>
+      <c r="AM21" s="74"/>
+      <c r="AN21" s="74"/>
+      <c r="AO21" s="74"/>
+      <c r="AP21" s="74"/>
+      <c r="AQ21" s="74"/>
+      <c r="AR21" s="74"/>
+      <c r="AS21" s="74"/>
+      <c r="AY21" s="79" t="s">
+        <v>207</v>
+      </c>
+      <c r="AZ21" s="79" t="s">
+        <v>381</v>
+      </c>
+      <c r="BA21" s="74"/>
+      <c r="BB21" s="79" t="s">
+        <v>299</v>
+      </c>
+      <c r="BC21" s="79" t="s">
+        <v>388</v>
+      </c>
+      <c r="BD21" s="74"/>
+      <c r="BE21" s="79" t="s">
+        <v>125</v>
+      </c>
+      <c r="BF21" s="79" t="s">
+        <v>392</v>
+      </c>
+      <c r="BI21" s="79" t="s">
+        <v>67</v>
+      </c>
+      <c r="BJ21" s="79" t="s">
+        <v>402</v>
+      </c>
+      <c r="BK21" s="74"/>
+      <c r="BL21" s="74"/>
+      <c r="BM21" s="74"/>
+    </row>
+    <row r="22" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A22" s="74"/>
+      <c r="K22" s="74"/>
+      <c r="L22" s="74"/>
+      <c r="M22" s="74"/>
+      <c r="N22" s="74"/>
+      <c r="O22" s="74"/>
+      <c r="P22" s="74"/>
+      <c r="Q22" s="74"/>
+      <c r="R22" s="74"/>
+      <c r="S22" s="74"/>
+      <c r="T22" s="74"/>
+      <c r="U22" s="74"/>
+      <c r="V22" s="74"/>
+      <c r="W22" s="74"/>
+      <c r="X22" s="74"/>
+      <c r="Y22" s="74"/>
+      <c r="Z22" s="74"/>
+      <c r="AA22" s="74"/>
+      <c r="AB22" s="74"/>
+      <c r="AC22" s="74"/>
+      <c r="AD22" s="74"/>
+      <c r="AE22" s="74"/>
+      <c r="AF22" s="74"/>
+      <c r="AG22" s="74"/>
+      <c r="AH22" s="74"/>
+      <c r="AI22" s="74"/>
+      <c r="AJ22" s="74"/>
+      <c r="AK22" s="74"/>
+      <c r="AL22" s="74"/>
+      <c r="AM22" s="74"/>
+      <c r="AN22" s="74"/>
+      <c r="AO22" s="74"/>
+      <c r="AP22" s="74"/>
+      <c r="AQ22" s="74"/>
+      <c r="AR22" s="74"/>
+      <c r="AS22" s="74"/>
+      <c r="AY22" s="79" t="s">
+        <v>126</v>
+      </c>
+      <c r="AZ22" s="79" t="s">
+        <v>382</v>
+      </c>
+      <c r="BA22" s="74"/>
+      <c r="BB22" s="74"/>
+      <c r="BC22" s="74"/>
+      <c r="BD22" s="74"/>
+      <c r="BE22" s="79" t="s">
+        <v>126</v>
+      </c>
+      <c r="BF22" s="79" t="s">
+        <v>393</v>
+      </c>
+      <c r="BI22" s="74"/>
+      <c r="BJ22" s="74"/>
+      <c r="BK22" s="74"/>
+      <c r="BL22" s="74"/>
+      <c r="BM22" s="74"/>
+    </row>
+    <row r="23" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="K23" s="74"/>
+      <c r="L23" s="74"/>
+      <c r="M23" s="74"/>
+      <c r="N23" s="74"/>
+      <c r="O23" s="74"/>
+      <c r="P23" s="74"/>
+      <c r="Q23" s="74"/>
+      <c r="R23" s="74"/>
+      <c r="S23" s="74"/>
+      <c r="T23" s="74"/>
+      <c r="U23" s="74"/>
+      <c r="V23" s="74"/>
+      <c r="W23" s="74"/>
+      <c r="X23" s="75"/>
+      <c r="Y23" s="74"/>
+      <c r="Z23" s="74"/>
+      <c r="AA23" s="74"/>
+      <c r="AB23" s="74"/>
+      <c r="AC23" s="74"/>
+      <c r="AD23" s="74"/>
+      <c r="AE23" s="74"/>
+      <c r="AF23" s="74"/>
+      <c r="AG23" s="74"/>
+      <c r="AH23" s="74"/>
+      <c r="AI23" s="74"/>
+      <c r="AJ23" s="74"/>
+      <c r="AK23" s="74"/>
+      <c r="AL23" s="74"/>
+      <c r="AM23" s="74"/>
+      <c r="AN23" s="74"/>
+      <c r="AO23" s="74"/>
+      <c r="AP23" s="74"/>
+      <c r="AQ23" s="74"/>
+      <c r="AR23" s="74"/>
+      <c r="AS23" s="74"/>
+      <c r="AU23" s="57"/>
+      <c r="BI23" s="74"/>
+      <c r="BJ23" s="74"/>
+      <c r="BK23" s="74"/>
+      <c r="BL23" s="74"/>
+      <c r="BM23" s="74"/>
+    </row>
+    <row r="24" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="K24" s="75"/>
+      <c r="L24" s="74"/>
+      <c r="M24" s="74"/>
+      <c r="N24" s="75"/>
+      <c r="O24" s="74"/>
+      <c r="P24" s="74"/>
+      <c r="Q24" s="75"/>
+      <c r="R24" s="74"/>
+      <c r="S24" s="74"/>
+      <c r="T24" s="74"/>
+      <c r="U24" s="74"/>
+      <c r="V24" s="74"/>
+      <c r="W24" s="74"/>
+      <c r="X24" s="74"/>
+      <c r="Y24" s="74"/>
+      <c r="Z24" s="74"/>
+      <c r="AA24" s="74"/>
+      <c r="AB24" s="74"/>
+      <c r="AD24" s="74"/>
+      <c r="AE24" s="74"/>
+      <c r="AF24" s="74"/>
+      <c r="AG24" s="74"/>
+      <c r="AH24" s="75"/>
+      <c r="AI24" s="74"/>
+      <c r="AJ24" s="74"/>
+      <c r="AK24" s="75"/>
+      <c r="AL24" s="74"/>
+      <c r="AM24" s="74"/>
+      <c r="AN24" s="74"/>
+      <c r="AO24" s="74"/>
+      <c r="AP24" s="74"/>
+      <c r="AQ24" s="74"/>
+      <c r="AR24" s="75"/>
+      <c r="AS24" s="74"/>
+      <c r="AY24" s="57"/>
+    </row>
+    <row r="25" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>406</v>
+      </c>
+      <c r="B25" t="s">
+        <v>407</v>
+      </c>
+      <c r="D25" s="75"/>
+      <c r="K25" s="74"/>
+      <c r="L25" s="74"/>
+      <c r="M25" s="74"/>
+      <c r="N25" s="74"/>
+      <c r="O25" s="74"/>
+      <c r="P25" s="74"/>
+      <c r="Q25" s="74"/>
+      <c r="R25" s="74"/>
+      <c r="S25" s="74"/>
+      <c r="T25" s="74"/>
+      <c r="U25" s="74"/>
+      <c r="V25" s="74"/>
+      <c r="W25" s="74"/>
+      <c r="X25" s="74"/>
+      <c r="Y25" s="74"/>
+      <c r="Z25" s="74"/>
+      <c r="AA25" s="74"/>
+      <c r="AB25" s="75"/>
+      <c r="AD25" s="74"/>
+      <c r="AE25" s="75"/>
+      <c r="AF25" s="74"/>
+      <c r="AG25" s="74"/>
+      <c r="AI25" s="74"/>
+      <c r="AJ25" s="74"/>
+      <c r="AK25" s="74"/>
+      <c r="AL25" s="74"/>
+      <c r="AM25" s="74"/>
+      <c r="AN25" s="74"/>
+      <c r="AO25" s="74"/>
+      <c r="AP25" s="74"/>
+      <c r="AQ25" s="74"/>
+      <c r="AR25" s="74"/>
+      <c r="AS25" s="74"/>
+      <c r="BI25" s="57"/>
+      <c r="BL25" s="57"/>
+    </row>
+    <row r="26" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>282</v>
+      </c>
+      <c r="B26" t="s">
+        <v>280</v>
+      </c>
+      <c r="K26" s="74"/>
+      <c r="L26" s="74"/>
+      <c r="M26" s="74"/>
+      <c r="N26" s="74"/>
+      <c r="O26" s="74"/>
+      <c r="P26" s="74"/>
+      <c r="Q26" s="74"/>
+      <c r="R26" s="74"/>
+      <c r="S26" s="74"/>
+      <c r="T26" s="74"/>
+      <c r="U26" s="74"/>
+      <c r="V26" s="74"/>
+      <c r="W26" s="74"/>
+      <c r="X26" s="74"/>
+      <c r="Y26" s="74"/>
+      <c r="Z26" s="74"/>
+      <c r="AA26" s="74"/>
+      <c r="AB26" s="74"/>
+      <c r="AC26" s="74"/>
+      <c r="AD26" s="74"/>
+      <c r="AE26" s="74"/>
+      <c r="AF26" s="74"/>
+      <c r="AG26" s="74"/>
+      <c r="AH26" s="74"/>
+      <c r="AI26" s="74"/>
+      <c r="AJ26" s="74"/>
+      <c r="AK26" s="74"/>
+      <c r="AL26" s="74"/>
+      <c r="AM26" s="74"/>
+      <c r="AN26" s="74"/>
+      <c r="AO26" s="74"/>
+      <c r="AP26" s="74"/>
+      <c r="AQ26" s="74"/>
+      <c r="AR26" s="74"/>
+      <c r="AS26" s="74"/>
+      <c r="BB26" s="57"/>
+      <c r="BE26" s="57"/>
+    </row>
+    <row r="27" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>306</v>
+      </c>
+      <c r="B27" t="s">
+        <v>284</v>
+      </c>
+      <c r="AC27" s="74"/>
+    </row>
+    <row r="28" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="29" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>322</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>344</v>
+      </c>
+      <c r="B31" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="32" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>361</v>
+      </c>
+      <c r="B32" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>363</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>376</v>
+      </c>
+      <c r="B35" t="s">
+        <v>398</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C364CD1-BD60-4795-8A34-8AD3606C6199}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11101,6 +14280,20 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7FC0B5A-8DF3-414E-B3BC-A3DB8B5A2D93}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -12025,8 +15218,8 @@
       <c r="J2" s="62"/>
       <c r="M2" s="59"/>
       <c r="N2" s="59"/>
-      <c r="O2" s="77"/>
-      <c r="P2" s="77"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="70">
@@ -12044,8 +15237,8 @@
       <c r="J3" s="62"/>
       <c r="M3" s="64"/>
       <c r="N3" s="64"/>
-      <c r="O3" s="77"/>
-      <c r="P3" s="77"/>
+      <c r="O3" s="88"/>
+      <c r="P3" s="88"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="70">
@@ -12063,8 +15256,8 @@
       <c r="J4" s="62"/>
       <c r="M4" s="64"/>
       <c r="N4" s="64"/>
-      <c r="O4" s="77"/>
-      <c r="P4" s="77"/>
+      <c r="O4" s="88"/>
+      <c r="P4" s="88"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="70">
@@ -12082,8 +15275,8 @@
       <c r="J5" s="62"/>
       <c r="M5" s="64"/>
       <c r="N5" s="64"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="77"/>
+      <c r="O5" s="88"/>
+      <c r="P5" s="88"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="70">
@@ -12101,8 +15294,8 @@
       <c r="J6" s="62"/>
       <c r="M6" s="64"/>
       <c r="N6" s="64"/>
-      <c r="O6" s="77"/>
-      <c r="P6" s="77"/>
+      <c r="O6" s="88"/>
+      <c r="P6" s="88"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="70">
@@ -12120,8 +15313,8 @@
       <c r="J7" s="62"/>
       <c r="M7" s="64"/>
       <c r="N7" s="64"/>
-      <c r="O7" s="77"/>
-      <c r="P7" s="77"/>
+      <c r="O7" s="88"/>
+      <c r="P7" s="88"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="70">
@@ -12139,8 +15332,8 @@
       <c r="J8" s="62"/>
       <c r="M8" s="64"/>
       <c r="N8" s="64"/>
-      <c r="O8" s="77"/>
-      <c r="P8" s="77"/>
+      <c r="O8" s="88"/>
+      <c r="P8" s="88"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="70">
@@ -12158,8 +15351,8 @@
       <c r="J9" s="62"/>
       <c r="M9" s="64"/>
       <c r="N9" s="64"/>
-      <c r="O9" s="77"/>
-      <c r="P9" s="77"/>
+      <c r="O9" s="88"/>
+      <c r="P9" s="88"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="62"/>
@@ -12171,8 +15364,8 @@
       <c r="J10" s="62"/>
       <c r="M10" s="64"/>
       <c r="N10" s="64"/>
-      <c r="O10" s="77"/>
-      <c r="P10" s="77"/>
+      <c r="O10" s="88"/>
+      <c r="P10" s="88"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="67" t="s">
@@ -12193,8 +15386,8 @@
       <c r="J11" s="62"/>
       <c r="M11" s="64"/>
       <c r="N11" s="64"/>
-      <c r="O11" s="77"/>
-      <c r="P11" s="77"/>
+      <c r="O11" s="88"/>
+      <c r="P11" s="88"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="70">
@@ -12215,8 +15408,8 @@
       <c r="J12" s="62"/>
       <c r="M12" s="64"/>
       <c r="N12" s="64"/>
-      <c r="O12" s="77"/>
-      <c r="P12" s="77"/>
+      <c r="O12" s="88"/>
+      <c r="P12" s="88"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="70">
@@ -12237,8 +15430,8 @@
       <c r="J13" s="62"/>
       <c r="M13" s="64"/>
       <c r="N13" s="61"/>
-      <c r="O13" s="77"/>
-      <c r="P13" s="77"/>
+      <c r="O13" s="88"/>
+      <c r="P13" s="88"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="70">

</xml_diff>